<commit_message>
Updated potentially eligible papers spreadsheet
</commit_message>
<xml_diff>
--- a/potentially_eligible_papers.xlsx
+++ b/potentially_eligible_papers.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E23388-62AA-4071-9E05-43BD1301AE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9C844B-4385-43F8-9365-4BD054849870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="1014">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="1015">
   <si>
     <t>Source</t>
   </si>
@@ -3159,12 +3159,15 @@
   <si>
     <t>JC, JLY, RD</t>
   </si>
+  <si>
+    <t>Google Scholar + Metas</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3243,8 +3246,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3289,8 +3299,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFD9EAD3"/>
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3321,7 +3337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3365,7 +3381,17 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3591,20 +3617,20 @@
   </sheetPr>
   <dimension ref="A1:Z423"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A386" workbookViewId="0">
+      <selection activeCell="C400" sqref="C400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" style="31" customWidth="1"/>
     <col min="2" max="2" width="37.7109375" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" customWidth="1"/>
     <col min="4" max="4" width="96.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="12.75">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3617,8 +3643,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" ht="12.75">
+      <c r="A2" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3631,9 +3657,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
+    <row r="3" spans="1:4" ht="12.75">
+      <c r="A3" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -3645,8 +3671,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" ht="12.75">
+      <c r="A4" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3659,8 +3685,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:4" ht="12.75">
+      <c r="A5" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -3673,8 +3699,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:4" ht="12.75">
+      <c r="A6" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -3687,8 +3713,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:4" ht="12.75">
+      <c r="A7" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -3701,8 +3727,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:4" ht="12.75">
+      <c r="A8" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -3715,8 +3741,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:4" ht="12.75">
+      <c r="A9" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3729,8 +3755,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:4" ht="12.75">
+      <c r="A10" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -3743,9 +3769,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
+    <row r="11" spans="1:4" ht="12.75">
+      <c r="A11" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>24</v>
@@ -3757,8 +3783,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:4" ht="12.75">
+      <c r="A12" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -3771,8 +3797,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:4" ht="12.75">
+      <c r="A13" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -3785,8 +3811,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:4" ht="12.75">
+      <c r="A14" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -3799,8 +3825,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:4" ht="12.75">
+      <c r="A15" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3813,8 +3839,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:4" ht="12.75">
+      <c r="A16" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -3827,8 +3853,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:4" ht="12.75">
+      <c r="A17" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -3841,8 +3867,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:4" ht="12.75">
+      <c r="A18" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -3855,8 +3881,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:4" ht="12.75">
+      <c r="A19" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -3869,8 +3895,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:4" ht="12.75">
+      <c r="A20" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -3883,9 +3909,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="2" t="s">
-        <v>7</v>
+    <row r="21" spans="1:4" ht="12.75">
+      <c r="A21" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>44</v>
@@ -3897,8 +3923,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:4" ht="12.75">
+      <c r="A22" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -3911,8 +3937,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:4" ht="12.75">
+      <c r="A23" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -3925,8 +3951,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:4" ht="12.75">
+      <c r="A24" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -3939,8 +3965,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:4" ht="12.75">
+      <c r="A25" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -3953,8 +3979,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:4" ht="12.75">
+      <c r="A26" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -3967,8 +3993,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:4" ht="12.75">
+      <c r="A27" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -3981,8 +4007,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:4" ht="12.75">
+      <c r="A28" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -3995,8 +4021,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:4" ht="12.75">
+      <c r="A29" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -4009,8 +4035,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:4" ht="12.75">
+      <c r="A30" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -4023,8 +4049,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:4" ht="12.75">
+      <c r="A31" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -4037,9 +4063,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="2" t="s">
-        <v>7</v>
+    <row r="32" spans="1:4" ht="12.75">
+      <c r="A32" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>67</v>
@@ -4051,8 +4077,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:4" ht="12.75">
+      <c r="A33" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -4065,8 +4091,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:4" ht="12.75">
+      <c r="A34" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -4079,8 +4105,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:4" ht="12.75">
+      <c r="A35" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -4093,8 +4119,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:4" ht="12.75">
+      <c r="A36" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -4107,8 +4133,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:4" ht="12.75">
+      <c r="A37" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -4121,8 +4147,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:4" ht="12.75">
+      <c r="A38" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -4135,8 +4161,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:4" ht="12.75">
+      <c r="A39" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -4149,8 +4175,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:4" ht="12.75">
+      <c r="A40" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -4163,8 +4189,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="2" t="s">
+    <row r="41" spans="1:4" ht="12.75">
+      <c r="A41" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -4177,8 +4203,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="2" t="s">
+    <row r="42" spans="1:4" ht="12.75">
+      <c r="A42" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -4191,8 +4217,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:4" ht="12.75">
+      <c r="A43" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -4205,8 +4231,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="4" t="s">
+    <row r="44" spans="1:4" ht="12.75">
+      <c r="A44" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -4219,9 +4245,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="2" t="s">
-        <v>7</v>
+    <row r="45" spans="1:4" ht="12.75">
+      <c r="A45" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>93</v>
@@ -4233,8 +4259,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="27" t="s">
+    <row r="46" spans="1:4" ht="12.75">
+      <c r="A46" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -4247,8 +4273,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="2" t="s">
+    <row r="47" spans="1:4" ht="12.75">
+      <c r="A47" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -4261,8 +4287,8 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="2" t="s">
+    <row r="48" spans="1:4" ht="12.75">
+      <c r="A48" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -4275,8 +4301,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="4" t="s">
+    <row r="49" spans="1:4" ht="12.75">
+      <c r="A49" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -4289,9 +4315,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="2" t="s">
-        <v>7</v>
+    <row r="50" spans="1:4" ht="12.75">
+      <c r="A50" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>103</v>
@@ -4303,8 +4329,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="2" t="s">
+    <row r="51" spans="1:4" ht="12.75">
+      <c r="A51" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -4317,8 +4343,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="4" t="s">
+    <row r="52" spans="1:4" ht="12.75">
+      <c r="A52" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -4331,8 +4357,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:4" ht="12.75">
+      <c r="A53" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -4345,9 +4371,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="2" t="s">
-        <v>7</v>
+    <row r="54" spans="1:4" ht="12.75">
+      <c r="A54" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>111</v>
@@ -4359,8 +4385,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="1:4" ht="12.75">
+      <c r="A55" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -4373,9 +4399,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="2" t="s">
-        <v>7</v>
+    <row r="56" spans="1:4" ht="12.75">
+      <c r="A56" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>115</v>
@@ -4387,8 +4413,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="4" t="s">
+    <row r="57" spans="1:4" ht="12.75">
+      <c r="A57" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -4401,8 +4427,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="2" t="s">
+    <row r="58" spans="1:4" ht="12.75">
+      <c r="A58" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -4415,8 +4441,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="2" t="s">
+    <row r="59" spans="1:4" ht="12.75">
+      <c r="A59" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -4429,8 +4455,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="2" t="s">
+    <row r="60" spans="1:4" ht="12.75">
+      <c r="A60" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -4443,8 +4469,8 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:4" ht="12.75">
+      <c r="A61" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -4457,8 +4483,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="4" t="s">
+    <row r="62" spans="1:4" ht="12.75">
+      <c r="A62" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -4471,8 +4497,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="2" t="s">
+    <row r="63" spans="1:4" ht="12.75">
+      <c r="A63" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -4485,8 +4511,8 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="2" t="s">
+    <row r="64" spans="1:4" ht="12.75">
+      <c r="A64" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -4499,8 +4525,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="4" t="s">
+    <row r="65" spans="1:4" ht="12.75">
+      <c r="A65" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -4513,8 +4539,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="2" t="s">
+    <row r="66" spans="1:4" ht="12.75">
+      <c r="A66" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -4527,8 +4553,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="4" t="s">
+    <row r="67" spans="1:4" ht="12.75">
+      <c r="A67" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -4541,8 +4567,8 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="2" t="s">
+    <row r="68" spans="1:4" ht="12.75">
+      <c r="A68" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -4555,8 +4581,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="4" t="s">
+    <row r="69" spans="1:4" ht="12.75">
+      <c r="A69" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -4569,8 +4595,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="4" t="s">
+    <row r="70" spans="1:4" ht="12.75">
+      <c r="A70" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -4583,8 +4609,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="4" t="s">
+    <row r="71" spans="1:4" ht="12.75">
+      <c r="A71" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B71" s="4" t="s">
@@ -4597,8 +4623,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="4" t="s">
+    <row r="72" spans="1:4" ht="12.75">
+      <c r="A72" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B72" s="4" t="s">
@@ -4611,9 +4637,9 @@
         <v>148</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="2" t="s">
-        <v>46</v>
+    <row r="73" spans="1:4" ht="12.75">
+      <c r="A73" s="28" t="s">
+        <v>1014</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>149</v>
@@ -4625,8 +4651,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="2" t="s">
+    <row r="74" spans="1:4" ht="12.75">
+      <c r="A74" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B74" s="2" t="s">
@@ -4639,9 +4665,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="2" t="s">
-        <v>7</v>
+    <row r="75" spans="1:4" ht="12.75">
+      <c r="A75" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>153</v>
@@ -4653,8 +4679,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="2" t="s">
+    <row r="76" spans="1:4" ht="12.75">
+      <c r="A76" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -4667,8 +4693,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="2" t="s">
+    <row r="77" spans="1:4" ht="12.75">
+      <c r="A77" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -4681,8 +4707,8 @@
         <v>158</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="2" t="s">
+    <row r="78" spans="1:4" ht="12.75">
+      <c r="A78" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -4695,8 +4721,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="4" t="s">
+    <row r="79" spans="1:4" ht="12.75">
+      <c r="A79" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B79" s="4" t="s">
@@ -4709,8 +4735,8 @@
         <v>162</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="4" t="s">
+    <row r="80" spans="1:4" ht="12.75">
+      <c r="A80" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B80" s="4" t="s">
@@ -4723,8 +4749,8 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="4" t="s">
+    <row r="81" spans="1:4" ht="12.75">
+      <c r="A81" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B81" s="4" t="s">
@@ -4737,8 +4763,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="4" t="s">
+    <row r="82" spans="1:4" ht="12.75">
+      <c r="A82" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B82" s="4" t="s">
@@ -4751,8 +4777,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="2" t="s">
+    <row r="83" spans="1:4" ht="12.75">
+      <c r="A83" s="30" t="s">
         <v>46</v>
       </c>
       <c r="B83" s="4" t="s">
@@ -4765,8 +4791,8 @@
         <v>170</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="4" t="s">
+    <row r="84" spans="1:4" ht="12.75">
+      <c r="A84" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B84" s="4" t="s">
@@ -4779,8 +4805,8 @@
         <v>172</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="4" t="s">
+    <row r="85" spans="1:4" ht="12.75">
+      <c r="A85" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B85" s="4" t="s">
@@ -4793,9 +4819,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="2" t="s">
-        <v>7</v>
+    <row r="86" spans="1:4" ht="12.75">
+      <c r="A86" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>175</v>
@@ -4807,8 +4833,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="4" t="s">
+    <row r="87" spans="1:4" ht="12.75">
+      <c r="A87" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B87" s="4" t="s">
@@ -4821,9 +4847,9 @@
         <v>178</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="2" t="s">
-        <v>46</v>
+    <row r="88" spans="1:4" ht="12.75">
+      <c r="A88" s="28" t="s">
+        <v>1014</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>179</v>
@@ -4835,8 +4861,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="4" t="s">
+    <row r="89" spans="1:4" ht="12.75">
+      <c r="A89" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B89" s="4" t="s">
@@ -4849,8 +4875,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="2" t="s">
+    <row r="90" spans="1:4" ht="12.75">
+      <c r="A90" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B90" s="2" t="s">
@@ -4863,8 +4889,8 @@
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="4" t="s">
+    <row r="91" spans="1:4" ht="12.75">
+      <c r="A91" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B91" s="4" t="s">
@@ -4877,8 +4903,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="2" t="s">
+    <row r="92" spans="1:4" ht="12.75">
+      <c r="A92" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B92" s="2" t="s">
@@ -4891,8 +4917,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="2" t="s">
+    <row r="93" spans="1:4" ht="12.75">
+      <c r="A93" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B93" s="2" t="s">
@@ -4905,8 +4931,8 @@
         <v>190</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="2" t="s">
+    <row r="94" spans="1:4" ht="12.75">
+      <c r="A94" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B94" s="2" t="s">
@@ -4919,8 +4945,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="2" t="s">
+    <row r="95" spans="1:4" ht="12.75">
+      <c r="A95" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B95" s="2" t="s">
@@ -4933,8 +4959,8 @@
         <v>194</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="2" t="s">
+    <row r="96" spans="1:4" ht="12.75">
+      <c r="A96" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B96" s="2" t="s">
@@ -4947,8 +4973,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="2" t="s">
+    <row r="97" spans="1:4" ht="12.75">
+      <c r="A97" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -4961,8 +4987,8 @@
         <v>198</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="4" t="s">
+    <row r="98" spans="1:4" ht="12.75">
+      <c r="A98" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B98" s="4" t="s">
@@ -4975,8 +5001,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="4" t="s">
+    <row r="99" spans="1:4" ht="12.75">
+      <c r="A99" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B99" s="4" t="s">
@@ -4989,8 +5015,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="2" t="s">
+    <row r="100" spans="1:4" ht="12.75">
+      <c r="A100" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B100" s="2" t="s">
@@ -5003,8 +5029,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="2" t="s">
+    <row r="101" spans="1:4" ht="12.75">
+      <c r="A101" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -5017,8 +5043,8 @@
         <v>206</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="2" t="s">
+    <row r="102" spans="1:4" ht="12.75">
+      <c r="A102" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="2" t="s">
@@ -5031,8 +5057,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="4" t="s">
+    <row r="103" spans="1:4" ht="12.75">
+      <c r="A103" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B103" s="5" t="s">
@@ -5045,8 +5071,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="2" t="s">
+    <row r="104" spans="1:4" ht="12.75">
+      <c r="A104" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B104" s="2" t="s">
@@ -5059,8 +5085,8 @@
         <v>212</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="2" t="s">
+    <row r="105" spans="1:4" ht="12.75">
+      <c r="A105" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B105" s="2" t="s">
@@ -5073,8 +5099,8 @@
         <v>214</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="4" t="s">
+    <row r="106" spans="1:4" ht="12.75">
+      <c r="A106" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B106" s="4" t="s">
@@ -5087,8 +5113,8 @@
         <v>216</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="2" t="s">
+    <row r="107" spans="1:4" ht="12.75">
+      <c r="A107" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B107" s="2" t="s">
@@ -5101,8 +5127,8 @@
         <v>218</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="2" t="s">
+    <row r="108" spans="1:4" ht="12.75">
+      <c r="A108" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B108" s="2" t="s">
@@ -5115,8 +5141,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="2" t="s">
+    <row r="109" spans="1:4" ht="12.75">
+      <c r="A109" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -5129,8 +5155,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="2" t="s">
+    <row r="110" spans="1:4" ht="12.75">
+      <c r="A110" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B110" s="2" t="s">
@@ -5143,8 +5169,8 @@
         <v>224</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="4" t="s">
+    <row r="111" spans="1:4" ht="12.75">
+      <c r="A111" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B111" s="4" t="s">
@@ -5157,8 +5183,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="27" t="s">
+    <row r="112" spans="1:4" ht="12.75">
+      <c r="A112" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B112" s="4" t="s">
@@ -5171,8 +5197,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="2" t="s">
+    <row r="113" spans="1:4" ht="12.75">
+      <c r="A113" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B113" s="2" t="s">
@@ -5185,9 +5211,9 @@
         <v>230</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="2" t="s">
-        <v>7</v>
+    <row r="114" spans="1:4" ht="12.75">
+      <c r="A114" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>231</v>
@@ -5199,8 +5225,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
-      <c r="A115" s="4" t="s">
+    <row r="115" spans="1:4" ht="12.75">
+      <c r="A115" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B115" s="4" t="s">
@@ -5213,8 +5239,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
-      <c r="A116" s="4" t="s">
+    <row r="116" spans="1:4" ht="12.75">
+      <c r="A116" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B116" s="4" t="s">
@@ -5227,8 +5253,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="4" t="s">
+    <row r="117" spans="1:4" ht="12.75">
+      <c r="A117" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B117" s="4" t="s">
@@ -5241,9 +5267,9 @@
         <v>238</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="2" t="s">
-        <v>7</v>
+    <row r="118" spans="1:4" ht="12.75">
+      <c r="A118" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>239</v>
@@ -5255,8 +5281,8 @@
         <v>240</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="2" t="s">
+    <row r="119" spans="1:4" ht="12.75">
+      <c r="A119" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B119" s="2" t="s">
@@ -5269,8 +5295,8 @@
         <v>242</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="2" t="s">
+    <row r="120" spans="1:4" ht="12.75">
+      <c r="A120" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B120" s="2" t="s">
@@ -5283,9 +5309,9 @@
         <v>244</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="2" t="s">
-        <v>7</v>
+    <row r="121" spans="1:4" ht="12.75">
+      <c r="A121" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>245</v>
@@ -5297,8 +5323,8 @@
         <v>246</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
-      <c r="A122" s="4" t="s">
+    <row r="122" spans="1:4" ht="12.75">
+      <c r="A122" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B122" s="4" t="s">
@@ -5311,8 +5337,8 @@
         <v>248</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
-      <c r="A123" s="2" t="s">
+    <row r="123" spans="1:4" ht="12.75">
+      <c r="A123" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B123" s="2" t="s">
@@ -5325,9 +5351,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
-      <c r="A124" s="2" t="s">
-        <v>7</v>
+    <row r="124" spans="1:4" ht="12.75">
+      <c r="A124" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>251</v>
@@ -5339,8 +5365,8 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
-      <c r="A125" s="4" t="s">
+    <row r="125" spans="1:4" ht="12.75">
+      <c r="A125" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B125" s="4" t="s">
@@ -5353,8 +5379,8 @@
         <v>254</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
-      <c r="A126" s="2" t="s">
+    <row r="126" spans="1:4" ht="12.75">
+      <c r="A126" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B126" s="2" t="s">
@@ -5367,9 +5393,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
-      <c r="A127" s="2" t="s">
-        <v>46</v>
+    <row r="127" spans="1:4" ht="12.75">
+      <c r="A127" s="28" t="s">
+        <v>1014</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>257</v>
@@ -5381,8 +5407,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
-      <c r="A128" s="4" t="s">
+    <row r="128" spans="1:4" ht="12.75">
+      <c r="A128" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B128" s="4" t="s">
@@ -5395,8 +5421,8 @@
         <v>260</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
-      <c r="A129" s="4" t="s">
+    <row r="129" spans="1:4" ht="12.75">
+      <c r="A129" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B129" s="4" t="s">
@@ -5409,8 +5435,8 @@
         <v>262</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
-      <c r="A130" s="2" t="s">
+    <row r="130" spans="1:4" ht="12.75">
+      <c r="A130" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B130" s="2" t="s">
@@ -5423,8 +5449,8 @@
         <v>264</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
-      <c r="A131" s="2" t="s">
+    <row r="131" spans="1:4" ht="12.75">
+      <c r="A131" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B131" s="2" t="s">
@@ -5437,8 +5463,8 @@
         <v>266</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
-      <c r="A132" s="2" t="s">
+    <row r="132" spans="1:4" ht="12.75">
+      <c r="A132" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B132" s="2" t="s">
@@ -5451,8 +5477,8 @@
         <v>268</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
-      <c r="A133" s="4" t="s">
+    <row r="133" spans="1:4" ht="12.75">
+      <c r="A133" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B133" s="4" t="s">
@@ -5465,8 +5491,8 @@
         <v>270</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
-      <c r="A134" s="2" t="s">
+    <row r="134" spans="1:4" ht="12.75">
+      <c r="A134" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B134" s="2" t="s">
@@ -5479,8 +5505,8 @@
         <v>272</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
-      <c r="A135" s="4" t="s">
+    <row r="135" spans="1:4" ht="12.75">
+      <c r="A135" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B135" s="4" t="s">
@@ -5493,8 +5519,8 @@
         <v>274</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
-      <c r="A136" s="4" t="s">
+    <row r="136" spans="1:4" ht="12.75">
+      <c r="A136" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B136" s="4" t="s">
@@ -5507,8 +5533,8 @@
         <v>276</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="4" t="s">
+    <row r="137" spans="1:4" ht="12.75">
+      <c r="A137" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B137" s="4" t="s">
@@ -5521,8 +5547,8 @@
         <v>278</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
-      <c r="A138" s="2" t="s">
+    <row r="138" spans="1:4" ht="12.75">
+      <c r="A138" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B138" s="2" t="s">
@@ -5535,8 +5561,8 @@
         <v>280</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
-      <c r="A139" s="4" t="s">
+    <row r="139" spans="1:4" ht="12.75">
+      <c r="A139" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B139" s="4" t="s">
@@ -5549,8 +5575,8 @@
         <v>282</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
-      <c r="A140" s="2" t="s">
+    <row r="140" spans="1:4" ht="12.75">
+      <c r="A140" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B140" s="2" t="s">
@@ -5563,8 +5589,8 @@
         <v>284</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
-      <c r="A141" s="2" t="s">
+    <row r="141" spans="1:4" ht="12.75">
+      <c r="A141" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B141" s="2" t="s">
@@ -5577,8 +5603,8 @@
         <v>286</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
-      <c r="A142" s="2" t="s">
+    <row r="142" spans="1:4" ht="12.75">
+      <c r="A142" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B142" s="2" t="s">
@@ -5591,8 +5617,8 @@
         <v>288</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
-      <c r="A143" s="2" t="s">
+    <row r="143" spans="1:4" ht="12.75">
+      <c r="A143" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B143" s="2" t="s">
@@ -5605,8 +5631,8 @@
         <v>290</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
-      <c r="A144" s="4" t="s">
+    <row r="144" spans="1:4" ht="12.75">
+      <c r="A144" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B144" s="4" t="s">
@@ -5619,8 +5645,8 @@
         <v>292</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
-      <c r="A145" s="2" t="s">
+    <row r="145" spans="1:4" ht="12.75">
+      <c r="A145" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B145" s="2" t="s">
@@ -5633,8 +5659,8 @@
         <v>294</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
-      <c r="A146" s="2" t="s">
+    <row r="146" spans="1:4" ht="12.75">
+      <c r="A146" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B146" s="2" t="s">
@@ -5647,8 +5673,8 @@
         <v>296</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
-      <c r="A147" s="4" t="s">
+    <row r="147" spans="1:4" ht="12.75">
+      <c r="A147" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B147" s="4" t="s">
@@ -5661,8 +5687,8 @@
         <v>298</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
-      <c r="A148" s="4" t="s">
+    <row r="148" spans="1:4" ht="12.75">
+      <c r="A148" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B148" s="4" t="s">
@@ -5675,9 +5701,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
-      <c r="A149" s="2" t="s">
-        <v>7</v>
+    <row r="149" spans="1:4" ht="12.75">
+      <c r="A149" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>301</v>
@@ -5689,8 +5715,8 @@
         <v>302</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
-      <c r="A150" s="2" t="s">
+    <row r="150" spans="1:4" ht="12.75">
+      <c r="A150" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B150" s="2" t="s">
@@ -5703,8 +5729,8 @@
         <v>304</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
-      <c r="A151" s="2" t="s">
+    <row r="151" spans="1:4" ht="12.75">
+      <c r="A151" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B151" s="2" t="s">
@@ -5717,8 +5743,8 @@
         <v>306</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
-      <c r="A152" s="4" t="s">
+    <row r="152" spans="1:4" ht="12.75">
+      <c r="A152" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B152" s="4" t="s">
@@ -5731,8 +5757,8 @@
         <v>308</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
-      <c r="A153" s="2" t="s">
+    <row r="153" spans="1:4" ht="12.75">
+      <c r="A153" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B153" s="2" t="s">
@@ -5745,8 +5771,8 @@
         <v>310</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
-      <c r="A154" s="4" t="s">
+    <row r="154" spans="1:4" ht="12.75">
+      <c r="A154" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B154" s="4" t="s">
@@ -5759,8 +5785,8 @@
         <v>312</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
-      <c r="A155" s="4" t="s">
+    <row r="155" spans="1:4" ht="12.75">
+      <c r="A155" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B155" s="4" t="s">
@@ -5773,8 +5799,8 @@
         <v>314</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
-      <c r="A156" s="2" t="s">
+    <row r="156" spans="1:4" ht="12.75">
+      <c r="A156" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B156" s="2" t="s">
@@ -5787,8 +5813,8 @@
         <v>316</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
-      <c r="A157" s="4" t="s">
+    <row r="157" spans="1:4" ht="12.75">
+      <c r="A157" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B157" s="4" t="s">
@@ -5801,8 +5827,8 @@
         <v>318</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
-      <c r="A158" s="2" t="s">
+    <row r="158" spans="1:4" ht="12.75">
+      <c r="A158" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B158" s="2" t="s">
@@ -5815,8 +5841,8 @@
         <v>320</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
-      <c r="A159" s="4" t="s">
+    <row r="159" spans="1:4" ht="12.75">
+      <c r="A159" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B159" s="4" t="s">
@@ -5829,8 +5855,8 @@
         <v>322</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
-      <c r="A160" s="2" t="s">
+    <row r="160" spans="1:4" ht="12.75">
+      <c r="A160" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B160" s="2" t="s">
@@ -5843,8 +5869,8 @@
         <v>324</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
-      <c r="A161" s="2" t="s">
+    <row r="161" spans="1:4" ht="12.75">
+      <c r="A161" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B161" s="2" t="s">
@@ -5857,8 +5883,8 @@
         <v>326</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
-      <c r="A162" s="4" t="s">
+    <row r="162" spans="1:4" ht="12.75">
+      <c r="A162" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B162" s="4" t="s">
@@ -5871,8 +5897,8 @@
         <v>328</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
-      <c r="A163" s="4" t="s">
+    <row r="163" spans="1:4" ht="12.75">
+      <c r="A163" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B163" s="4" t="s">
@@ -5885,8 +5911,8 @@
         <v>330</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
-      <c r="A164" s="2" t="s">
+    <row r="164" spans="1:4" ht="12.75">
+      <c r="A164" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B164" s="2" t="s">
@@ -5899,8 +5925,8 @@
         <v>332</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
-      <c r="A165" s="4" t="s">
+    <row r="165" spans="1:4" ht="12.75">
+      <c r="A165" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B165" s="4" t="s">
@@ -5913,8 +5939,8 @@
         <v>334</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
-      <c r="A166" s="2" t="s">
+    <row r="166" spans="1:4" ht="12.75">
+      <c r="A166" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B166" s="2" t="s">
@@ -5927,8 +5953,8 @@
         <v>336</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
-      <c r="A167" s="4" t="s">
+    <row r="167" spans="1:4" ht="12.75">
+      <c r="A167" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B167" s="4" t="s">
@@ -5941,8 +5967,8 @@
         <v>338</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
-      <c r="A168" s="4" t="s">
+    <row r="168" spans="1:4" ht="12.75">
+      <c r="A168" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B168" s="4" t="s">
@@ -5955,8 +5981,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
-      <c r="A169" s="4" t="s">
+    <row r="169" spans="1:4" ht="12.75">
+      <c r="A169" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B169" s="4" t="s">
@@ -5969,8 +5995,8 @@
         <v>342</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
-      <c r="A170" s="4" t="s">
+    <row r="170" spans="1:4" ht="12.75">
+      <c r="A170" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B170" s="4" t="s">
@@ -5983,8 +6009,8 @@
         <v>344</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
-      <c r="A171" s="4" t="s">
+    <row r="171" spans="1:4" ht="12.75">
+      <c r="A171" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B171" s="4" t="s">
@@ -5997,8 +6023,8 @@
         <v>346</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
-      <c r="A172" s="2" t="s">
+    <row r="172" spans="1:4" ht="12.75">
+      <c r="A172" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B172" s="2" t="s">
@@ -6011,8 +6037,8 @@
         <v>348</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
-      <c r="A173" s="4" t="s">
+    <row r="173" spans="1:4" ht="12.75">
+      <c r="A173" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B173" s="4" t="s">
@@ -6025,8 +6051,8 @@
         <v>350</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
-      <c r="A174" s="4" t="s">
+    <row r="174" spans="1:4" ht="12.75">
+      <c r="A174" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B174" s="4" t="s">
@@ -6039,8 +6065,8 @@
         <v>352</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
-      <c r="A175" s="4" t="s">
+    <row r="175" spans="1:4" ht="12.75">
+      <c r="A175" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B175" s="4" t="s">
@@ -6053,8 +6079,8 @@
         <v>354</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
-      <c r="A176" s="4" t="s">
+    <row r="176" spans="1:4" ht="12.75">
+      <c r="A176" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B176" s="4" t="s">
@@ -6067,9 +6093,9 @@
         <v>356</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
-      <c r="A177" s="2" t="s">
-        <v>7</v>
+    <row r="177" spans="1:4" ht="12.75">
+      <c r="A177" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>357</v>
@@ -6081,8 +6107,8 @@
         <v>358</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
-      <c r="A178" s="2" t="s">
+    <row r="178" spans="1:4" ht="12.75">
+      <c r="A178" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B178" s="2" t="s">
@@ -6095,8 +6121,8 @@
         <v>360</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
-      <c r="A179" s="4" t="s">
+    <row r="179" spans="1:4" ht="12.75">
+      <c r="A179" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B179" s="4" t="s">
@@ -6109,8 +6135,8 @@
         <v>362</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
-      <c r="A180" s="4" t="s">
+    <row r="180" spans="1:4" ht="12.75">
+      <c r="A180" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B180" s="4" t="s">
@@ -6123,8 +6149,8 @@
         <v>364</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
-      <c r="A181" s="4" t="s">
+    <row r="181" spans="1:4" ht="12.75">
+      <c r="A181" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B181" s="4" t="s">
@@ -6137,8 +6163,8 @@
         <v>366</v>
       </c>
     </row>
-    <row r="182" spans="1:4">
-      <c r="A182" s="4" t="s">
+    <row r="182" spans="1:4" ht="12.75">
+      <c r="A182" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B182" s="4" t="s">
@@ -6151,8 +6177,8 @@
         <v>368</v>
       </c>
     </row>
-    <row r="183" spans="1:4">
-      <c r="A183" s="4" t="s">
+    <row r="183" spans="1:4" ht="12.75">
+      <c r="A183" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B183" s="5" t="s">
@@ -6165,8 +6191,8 @@
         <v>370</v>
       </c>
     </row>
-    <row r="184" spans="1:4">
-      <c r="A184" s="4" t="s">
+    <row r="184" spans="1:4" ht="12.75">
+      <c r="A184" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B184" s="4" t="s">
@@ -6179,8 +6205,8 @@
         <v>372</v>
       </c>
     </row>
-    <row r="185" spans="1:4">
-      <c r="A185" s="2" t="s">
+    <row r="185" spans="1:4" ht="12.75">
+      <c r="A185" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B185" s="2" t="s">
@@ -6193,8 +6219,8 @@
         <v>374</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
-      <c r="A186" s="4" t="s">
+    <row r="186" spans="1:4" ht="12.75">
+      <c r="A186" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B186" s="4" t="s">
@@ -6207,8 +6233,8 @@
         <v>376</v>
       </c>
     </row>
-    <row r="187" spans="1:4">
-      <c r="A187" s="4" t="s">
+    <row r="187" spans="1:4" ht="12.75">
+      <c r="A187" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B187" s="4" t="s">
@@ -6221,8 +6247,8 @@
         <v>378</v>
       </c>
     </row>
-    <row r="188" spans="1:4">
-      <c r="A188" s="2" t="s">
+    <row r="188" spans="1:4" ht="12.75">
+      <c r="A188" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B188" s="2" t="s">
@@ -6235,8 +6261,8 @@
         <v>380</v>
       </c>
     </row>
-    <row r="189" spans="1:4">
-      <c r="A189" s="4" t="s">
+    <row r="189" spans="1:4" ht="12.75">
+      <c r="A189" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B189" s="4" t="s">
@@ -6249,8 +6275,8 @@
         <v>382</v>
       </c>
     </row>
-    <row r="190" spans="1:4">
-      <c r="A190" s="4" t="s">
+    <row r="190" spans="1:4" ht="12.75">
+      <c r="A190" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B190" s="4" t="s">
@@ -6263,8 +6289,8 @@
         <v>384</v>
       </c>
     </row>
-    <row r="191" spans="1:4">
-      <c r="A191" s="2" t="s">
+    <row r="191" spans="1:4" ht="12.75">
+      <c r="A191" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B191" s="2" t="s">
@@ -6277,8 +6303,8 @@
         <v>386</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
-      <c r="A192" s="2" t="s">
+    <row r="192" spans="1:4" ht="12.75">
+      <c r="A192" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B192" s="2" t="s">
@@ -6291,8 +6317,8 @@
         <v>388</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
-      <c r="A193" s="2" t="s">
+    <row r="193" spans="1:4" ht="12.75">
+      <c r="A193" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B193" s="2" t="s">
@@ -6305,8 +6331,8 @@
         <v>390</v>
       </c>
     </row>
-    <row r="194" spans="1:4">
-      <c r="A194" s="4" t="s">
+    <row r="194" spans="1:4" ht="12.75">
+      <c r="A194" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B194" s="4" t="s">
@@ -6319,8 +6345,8 @@
         <v>392</v>
       </c>
     </row>
-    <row r="195" spans="1:4">
-      <c r="A195" s="2" t="s">
+    <row r="195" spans="1:4" ht="12.75">
+      <c r="A195" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B195" s="2" t="s">
@@ -6333,8 +6359,8 @@
         <v>394</v>
       </c>
     </row>
-    <row r="196" spans="1:4">
-      <c r="A196" s="4" t="s">
+    <row r="196" spans="1:4" ht="12.75">
+      <c r="A196" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B196" s="4" t="s">
@@ -6347,8 +6373,8 @@
         <v>396</v>
       </c>
     </row>
-    <row r="197" spans="1:4">
-      <c r="A197" s="2" t="s">
+    <row r="197" spans="1:4" ht="12.75">
+      <c r="A197" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B197" s="2" t="s">
@@ -6361,8 +6387,8 @@
         <v>398</v>
       </c>
     </row>
-    <row r="198" spans="1:4">
-      <c r="A198" s="4" t="s">
+    <row r="198" spans="1:4" ht="12.75">
+      <c r="A198" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B198" s="4" t="s">
@@ -6375,8 +6401,8 @@
         <v>400</v>
       </c>
     </row>
-    <row r="199" spans="1:4">
-      <c r="A199" s="4" t="s">
+    <row r="199" spans="1:4" ht="12.75">
+      <c r="A199" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B199" s="4" t="s">
@@ -6389,8 +6415,8 @@
         <v>402</v>
       </c>
     </row>
-    <row r="200" spans="1:4">
-      <c r="A200" s="2" t="s">
+    <row r="200" spans="1:4" ht="12.75">
+      <c r="A200" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B200" s="2" t="s">
@@ -6403,8 +6429,8 @@
         <v>404</v>
       </c>
     </row>
-    <row r="201" spans="1:4">
-      <c r="A201" s="4" t="s">
+    <row r="201" spans="1:4" ht="12.75">
+      <c r="A201" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B201" s="4" t="s">
@@ -6417,8 +6443,8 @@
         <v>406</v>
       </c>
     </row>
-    <row r="202" spans="1:4">
-      <c r="A202" s="4" t="s">
+    <row r="202" spans="1:4" ht="12.75">
+      <c r="A202" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B202" s="4" t="s">
@@ -6431,9 +6457,9 @@
         <v>408</v>
       </c>
     </row>
-    <row r="203" spans="1:4">
-      <c r="A203" s="2" t="s">
-        <v>46</v>
+    <row r="203" spans="1:4" ht="12.75">
+      <c r="A203" s="28" t="s">
+        <v>1014</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>409</v>
@@ -6445,8 +6471,8 @@
         <v>410</v>
       </c>
     </row>
-    <row r="204" spans="1:4">
-      <c r="A204" s="4" t="s">
+    <row r="204" spans="1:4" ht="12.75">
+      <c r="A204" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B204" s="4" t="s">
@@ -6459,8 +6485,8 @@
         <v>412</v>
       </c>
     </row>
-    <row r="205" spans="1:4">
-      <c r="A205" s="4" t="s">
+    <row r="205" spans="1:4" ht="12.75">
+      <c r="A205" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B205" s="4" t="s">
@@ -6473,8 +6499,8 @@
         <v>414</v>
       </c>
     </row>
-    <row r="206" spans="1:4">
-      <c r="A206" s="4" t="s">
+    <row r="206" spans="1:4" ht="12.75">
+      <c r="A206" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B206" s="4" t="s">
@@ -6487,8 +6513,8 @@
         <v>416</v>
       </c>
     </row>
-    <row r="207" spans="1:4">
-      <c r="A207" s="4" t="s">
+    <row r="207" spans="1:4" ht="12.75">
+      <c r="A207" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B207" s="4" t="s">
@@ -6501,8 +6527,8 @@
         <v>418</v>
       </c>
     </row>
-    <row r="208" spans="1:4">
-      <c r="A208" s="4" t="s">
+    <row r="208" spans="1:4" ht="12.75">
+      <c r="A208" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B208" s="4" t="s">
@@ -6515,8 +6541,8 @@
         <v>420</v>
       </c>
     </row>
-    <row r="209" spans="1:4">
-      <c r="A209" s="4" t="s">
+    <row r="209" spans="1:4" ht="12.75">
+      <c r="A209" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B209" s="4" t="s">
@@ -6529,8 +6555,8 @@
         <v>422</v>
       </c>
     </row>
-    <row r="210" spans="1:4">
-      <c r="A210" s="4" t="s">
+    <row r="210" spans="1:4" ht="12.75">
+      <c r="A210" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B210" s="4" t="s">
@@ -6543,8 +6569,8 @@
         <v>424</v>
       </c>
     </row>
-    <row r="211" spans="1:4">
-      <c r="A211" s="4" t="s">
+    <row r="211" spans="1:4" ht="12.75">
+      <c r="A211" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B211" s="4" t="s">
@@ -6557,8 +6583,8 @@
         <v>425</v>
       </c>
     </row>
-    <row r="212" spans="1:4">
-      <c r="A212" s="2" t="s">
+    <row r="212" spans="1:4" ht="12.75">
+      <c r="A212" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B212" s="2" t="s">
@@ -6571,8 +6597,8 @@
         <v>427</v>
       </c>
     </row>
-    <row r="213" spans="1:4">
-      <c r="A213" s="4" t="s">
+    <row r="213" spans="1:4" ht="12.75">
+      <c r="A213" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B213" s="4" t="s">
@@ -6585,8 +6611,8 @@
         <v>429</v>
       </c>
     </row>
-    <row r="214" spans="1:4">
-      <c r="A214" s="4" t="s">
+    <row r="214" spans="1:4" ht="12.75">
+      <c r="A214" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B214" s="4" t="s">
@@ -6599,8 +6625,8 @@
         <v>431</v>
       </c>
     </row>
-    <row r="215" spans="1:4">
-      <c r="A215" s="4" t="s">
+    <row r="215" spans="1:4" ht="12.75">
+      <c r="A215" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B215" s="4" t="s">
@@ -6613,8 +6639,8 @@
         <v>433</v>
       </c>
     </row>
-    <row r="216" spans="1:4">
-      <c r="A216" s="4" t="s">
+    <row r="216" spans="1:4" ht="12.75">
+      <c r="A216" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B216" s="4" t="s">
@@ -6627,8 +6653,8 @@
         <v>434</v>
       </c>
     </row>
-    <row r="217" spans="1:4">
-      <c r="A217" s="4" t="s">
+    <row r="217" spans="1:4" ht="12.75">
+      <c r="A217" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B217" s="4" t="s">
@@ -6641,8 +6667,8 @@
         <v>436</v>
       </c>
     </row>
-    <row r="218" spans="1:4">
-      <c r="A218" s="27" t="s">
+    <row r="218" spans="1:4" ht="12.75">
+      <c r="A218" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B218" s="4" t="s">
@@ -6655,9 +6681,9 @@
         <v>438</v>
       </c>
     </row>
-    <row r="219" spans="1:4">
-      <c r="A219" s="2" t="s">
-        <v>7</v>
+    <row r="219" spans="1:4" ht="12.75">
+      <c r="A219" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>439</v>
@@ -6669,8 +6695,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="220" spans="1:4">
-      <c r="A220" s="2" t="s">
+    <row r="220" spans="1:4" ht="12.75">
+      <c r="A220" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B220" s="2" t="s">
@@ -6683,8 +6709,8 @@
         <v>442</v>
       </c>
     </row>
-    <row r="221" spans="1:4">
-      <c r="A221" s="4" t="s">
+    <row r="221" spans="1:4" ht="12.75">
+      <c r="A221" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B221" s="4" t="s">
@@ -6697,8 +6723,8 @@
         <v>444</v>
       </c>
     </row>
-    <row r="222" spans="1:4">
-      <c r="A222" s="4" t="s">
+    <row r="222" spans="1:4" ht="12.75">
+      <c r="A222" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B222" s="4" t="s">
@@ -6711,8 +6737,8 @@
         <v>446</v>
       </c>
     </row>
-    <row r="223" spans="1:4">
-      <c r="A223" s="2" t="s">
+    <row r="223" spans="1:4" ht="12.75">
+      <c r="A223" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B223" s="2" t="s">
@@ -6725,8 +6751,8 @@
         <v>448</v>
       </c>
     </row>
-    <row r="224" spans="1:4">
-      <c r="A224" s="4" t="s">
+    <row r="224" spans="1:4" ht="12.75">
+      <c r="A224" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B224" s="4" t="s">
@@ -6739,8 +6765,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="225" spans="1:4">
-      <c r="A225" s="4" t="s">
+    <row r="225" spans="1:4" ht="12.75">
+      <c r="A225" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B225" s="4" t="s">
@@ -6753,8 +6779,8 @@
         <v>452</v>
       </c>
     </row>
-    <row r="226" spans="1:4">
-      <c r="A226" s="4" t="s">
+    <row r="226" spans="1:4" ht="12.75">
+      <c r="A226" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B226" s="4" t="s">
@@ -6767,8 +6793,8 @@
         <v>454</v>
       </c>
     </row>
-    <row r="227" spans="1:4">
-      <c r="A227" s="4" t="s">
+    <row r="227" spans="1:4" ht="12.75">
+      <c r="A227" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B227" s="4" t="s">
@@ -6781,8 +6807,8 @@
         <v>456</v>
       </c>
     </row>
-    <row r="228" spans="1:4">
-      <c r="A228" s="2" t="s">
+    <row r="228" spans="1:4" ht="12.75">
+      <c r="A228" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B228" s="2" t="s">
@@ -6795,8 +6821,8 @@
         <v>458</v>
       </c>
     </row>
-    <row r="229" spans="1:4">
-      <c r="A229" s="4" t="s">
+    <row r="229" spans="1:4" ht="12.75">
+      <c r="A229" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B229" s="4" t="s">
@@ -6809,9 +6835,9 @@
         <v>460</v>
       </c>
     </row>
-    <row r="230" spans="1:4">
-      <c r="A230" s="2" t="s">
-        <v>7</v>
+    <row r="230" spans="1:4" ht="12.75">
+      <c r="A230" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>461</v>
@@ -6823,8 +6849,8 @@
         <v>462</v>
       </c>
     </row>
-    <row r="231" spans="1:4">
-      <c r="A231" s="4" t="s">
+    <row r="231" spans="1:4" ht="12.75">
+      <c r="A231" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B231" s="4" t="s">
@@ -6837,8 +6863,8 @@
         <v>464</v>
       </c>
     </row>
-    <row r="232" spans="1:4">
-      <c r="A232" s="2" t="s">
+    <row r="232" spans="1:4" ht="12.75">
+      <c r="A232" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B232" s="2" t="s">
@@ -6851,8 +6877,8 @@
         <v>466</v>
       </c>
     </row>
-    <row r="233" spans="1:4">
-      <c r="A233" s="2" t="s">
+    <row r="233" spans="1:4" ht="12.75">
+      <c r="A233" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B233" s="2" t="s">
@@ -6865,8 +6891,8 @@
         <v>468</v>
       </c>
     </row>
-    <row r="234" spans="1:4">
-      <c r="A234" s="27" t="s">
+    <row r="234" spans="1:4" ht="12.75">
+      <c r="A234" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B234" s="4" t="s">
@@ -6879,8 +6905,8 @@
         <v>470</v>
       </c>
     </row>
-    <row r="235" spans="1:4">
-      <c r="A235" s="4" t="s">
+    <row r="235" spans="1:4" ht="12.75">
+      <c r="A235" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B235" s="4" t="s">
@@ -6893,8 +6919,8 @@
         <v>471</v>
       </c>
     </row>
-    <row r="236" spans="1:4">
-      <c r="A236" s="4" t="s">
+    <row r="236" spans="1:4" ht="12.75">
+      <c r="A236" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B236" s="4" t="s">
@@ -6907,8 +6933,8 @@
         <v>473</v>
       </c>
     </row>
-    <row r="237" spans="1:4">
-      <c r="A237" s="4" t="s">
+    <row r="237" spans="1:4" ht="12.75">
+      <c r="A237" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B237" s="4" t="s">
@@ -6921,8 +6947,8 @@
         <v>475</v>
       </c>
     </row>
-    <row r="238" spans="1:4">
-      <c r="A238" s="4" t="s">
+    <row r="238" spans="1:4" ht="12.75">
+      <c r="A238" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B238" s="4" t="s">
@@ -6935,8 +6961,8 @@
         <v>477</v>
       </c>
     </row>
-    <row r="239" spans="1:4">
-      <c r="A239" s="2" t="s">
+    <row r="239" spans="1:4" ht="12.75">
+      <c r="A239" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B239" s="2" t="s">
@@ -6949,8 +6975,8 @@
         <v>479</v>
       </c>
     </row>
-    <row r="240" spans="1:4">
-      <c r="A240" s="2" t="s">
+    <row r="240" spans="1:4" ht="12.75">
+      <c r="A240" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B240" s="2" t="s">
@@ -6963,8 +6989,8 @@
         <v>481</v>
       </c>
     </row>
-    <row r="241" spans="1:4">
-      <c r="A241" s="4" t="s">
+    <row r="241" spans="1:4" ht="12.75">
+      <c r="A241" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B241" s="4" t="s">
@@ -6977,8 +7003,8 @@
         <v>483</v>
       </c>
     </row>
-    <row r="242" spans="1:4">
-      <c r="A242" s="4" t="s">
+    <row r="242" spans="1:4" ht="12.75">
+      <c r="A242" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B242" s="4" t="s">
@@ -6991,8 +7017,8 @@
         <v>485</v>
       </c>
     </row>
-    <row r="243" spans="1:4">
-      <c r="A243" s="4" t="s">
+    <row r="243" spans="1:4" ht="12.75">
+      <c r="A243" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B243" s="4" t="s">
@@ -7005,8 +7031,8 @@
         <v>487</v>
       </c>
     </row>
-    <row r="244" spans="1:4">
-      <c r="A244" s="4" t="s">
+    <row r="244" spans="1:4" ht="12.75">
+      <c r="A244" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B244" s="4" t="s">
@@ -7019,8 +7045,8 @@
         <v>489</v>
       </c>
     </row>
-    <row r="245" spans="1:4">
-      <c r="A245" s="4" t="s">
+    <row r="245" spans="1:4" ht="12.75">
+      <c r="A245" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B245" s="4" t="s">
@@ -7033,8 +7059,8 @@
         <v>491</v>
       </c>
     </row>
-    <row r="246" spans="1:4">
-      <c r="A246" s="2" t="s">
+    <row r="246" spans="1:4" ht="12.75">
+      <c r="A246" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B246" s="2" t="s">
@@ -7047,8 +7073,8 @@
         <v>493</v>
       </c>
     </row>
-    <row r="247" spans="1:4">
-      <c r="A247" s="4" t="s">
+    <row r="247" spans="1:4" ht="12.75">
+      <c r="A247" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B247" s="4" t="s">
@@ -7061,9 +7087,9 @@
         <v>495</v>
       </c>
     </row>
-    <row r="248" spans="1:4">
-      <c r="A248" s="2" t="s">
-        <v>46</v>
+    <row r="248" spans="1:4" ht="12.75">
+      <c r="A248" s="28" t="s">
+        <v>1014</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>496</v>
@@ -7075,8 +7101,8 @@
         <v>497</v>
       </c>
     </row>
-    <row r="249" spans="1:4">
-      <c r="A249" s="4" t="s">
+    <row r="249" spans="1:4" ht="12.75">
+      <c r="A249" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B249" s="4" t="s">
@@ -7089,8 +7115,8 @@
         <v>499</v>
       </c>
     </row>
-    <row r="250" spans="1:4">
-      <c r="A250" s="2" t="s">
+    <row r="250" spans="1:4" ht="12.75">
+      <c r="A250" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
@@ -7103,8 +7129,8 @@
         <v>501</v>
       </c>
     </row>
-    <row r="251" spans="1:4">
-      <c r="A251" s="2" t="s">
+    <row r="251" spans="1:4" ht="12.75">
+      <c r="A251" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B251" s="2" t="s">
@@ -7117,8 +7143,8 @@
         <v>503</v>
       </c>
     </row>
-    <row r="252" spans="1:4">
-      <c r="A252" s="4" t="s">
+    <row r="252" spans="1:4" ht="12.75">
+      <c r="A252" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B252" s="4" t="s">
@@ -7131,8 +7157,8 @@
         <v>505</v>
       </c>
     </row>
-    <row r="253" spans="1:4">
-      <c r="A253" s="4" t="s">
+    <row r="253" spans="1:4" ht="12.75">
+      <c r="A253" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B253" s="4" t="s">
@@ -7145,8 +7171,8 @@
         <v>280</v>
       </c>
     </row>
-    <row r="254" spans="1:4">
-      <c r="A254" s="4" t="s">
+    <row r="254" spans="1:4" ht="12.75">
+      <c r="A254" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B254" s="4" t="s">
@@ -7159,8 +7185,8 @@
         <v>507</v>
       </c>
     </row>
-    <row r="255" spans="1:4">
-      <c r="A255" s="2" t="s">
+    <row r="255" spans="1:4" ht="12.75">
+      <c r="A255" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B255" s="2" t="s">
@@ -7173,8 +7199,8 @@
         <v>509</v>
       </c>
     </row>
-    <row r="256" spans="1:4">
-      <c r="A256" s="4" t="s">
+    <row r="256" spans="1:4" ht="12.75">
+      <c r="A256" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B256" s="4" t="s">
@@ -7187,8 +7213,8 @@
         <v>511</v>
       </c>
     </row>
-    <row r="257" spans="1:4">
-      <c r="A257" s="2" t="s">
+    <row r="257" spans="1:4" ht="12.75">
+      <c r="A257" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B257" s="2" t="s">
@@ -7201,8 +7227,8 @@
         <v>513</v>
       </c>
     </row>
-    <row r="258" spans="1:4">
-      <c r="A258" s="4" t="s">
+    <row r="258" spans="1:4" ht="12.75">
+      <c r="A258" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B258" s="4" t="s">
@@ -7215,8 +7241,8 @@
         <v>515</v>
       </c>
     </row>
-    <row r="259" spans="1:4">
-      <c r="A259" s="4" t="s">
+    <row r="259" spans="1:4" ht="12.75">
+      <c r="A259" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B259" s="4" t="s">
@@ -7229,8 +7255,8 @@
         <v>517</v>
       </c>
     </row>
-    <row r="260" spans="1:4">
-      <c r="A260" s="4" t="s">
+    <row r="260" spans="1:4" ht="12.75">
+      <c r="A260" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B260" s="4" t="s">
@@ -7243,8 +7269,8 @@
         <v>519</v>
       </c>
     </row>
-    <row r="261" spans="1:4">
-      <c r="A261" s="4" t="s">
+    <row r="261" spans="1:4" ht="12.75">
+      <c r="A261" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B261" s="4" t="s">
@@ -7257,8 +7283,8 @@
         <v>521</v>
       </c>
     </row>
-    <row r="262" spans="1:4">
-      <c r="A262" s="4" t="s">
+    <row r="262" spans="1:4" ht="12.75">
+      <c r="A262" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B262" s="4" t="s">
@@ -7271,8 +7297,8 @@
         <v>523</v>
       </c>
     </row>
-    <row r="263" spans="1:4">
-      <c r="A263" s="4" t="s">
+    <row r="263" spans="1:4" ht="12.75">
+      <c r="A263" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B263" s="4" t="s">
@@ -7285,8 +7311,8 @@
         <v>525</v>
       </c>
     </row>
-    <row r="264" spans="1:4">
-      <c r="A264" s="4" t="s">
+    <row r="264" spans="1:4" ht="12.75">
+      <c r="A264" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B264" s="4" t="s">
@@ -7299,8 +7325,8 @@
         <v>527</v>
       </c>
     </row>
-    <row r="265" spans="1:4">
-      <c r="A265" s="4" t="s">
+    <row r="265" spans="1:4" ht="12.75">
+      <c r="A265" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B265" s="4" t="s">
@@ -7313,8 +7339,8 @@
         <v>529</v>
       </c>
     </row>
-    <row r="266" spans="1:4">
-      <c r="A266" s="2" t="s">
+    <row r="266" spans="1:4" ht="12.75">
+      <c r="A266" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B266" s="2" t="s">
@@ -7327,8 +7353,8 @@
         <v>532</v>
       </c>
     </row>
-    <row r="267" spans="1:4">
-      <c r="A267" s="2" t="s">
+    <row r="267" spans="1:4" ht="12.75">
+      <c r="A267" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B267" s="2" t="s">
@@ -7341,8 +7367,8 @@
         <v>535</v>
       </c>
     </row>
-    <row r="268" spans="1:4">
-      <c r="A268" s="4" t="s">
+    <row r="268" spans="1:4" ht="12.75">
+      <c r="A268" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B268" s="4" t="s">
@@ -7355,8 +7381,8 @@
         <v>537</v>
       </c>
     </row>
-    <row r="269" spans="1:4">
-      <c r="A269" s="2" t="s">
+    <row r="269" spans="1:4" ht="12.75">
+      <c r="A269" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B269" s="2" t="s">
@@ -7369,8 +7395,8 @@
         <v>539</v>
       </c>
     </row>
-    <row r="270" spans="1:4">
-      <c r="A270" s="26" t="s">
+    <row r="270" spans="1:4" ht="12.75">
+      <c r="A270" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B270" s="7" t="s">
@@ -7383,8 +7409,8 @@
         <v>541</v>
       </c>
     </row>
-    <row r="271" spans="1:4">
-      <c r="A271" s="2" t="s">
+    <row r="271" spans="1:4" ht="12.75">
+      <c r="A271" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B271" s="8" t="s">
@@ -7397,8 +7423,8 @@
         <v>543</v>
       </c>
     </row>
-    <row r="272" spans="1:4">
-      <c r="A272" s="2" t="s">
+    <row r="272" spans="1:4" ht="12.75">
+      <c r="A272" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B272" s="8" t="s">
@@ -7411,8 +7437,8 @@
         <v>545</v>
       </c>
     </row>
-    <row r="273" spans="1:4">
-      <c r="A273" s="4" t="s">
+    <row r="273" spans="1:4" ht="12.75">
+      <c r="A273" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B273" s="5" t="s">
@@ -7425,8 +7451,8 @@
         <v>547</v>
       </c>
     </row>
-    <row r="274" spans="1:4">
-      <c r="A274" s="2" t="s">
+    <row r="274" spans="1:4" ht="12.75">
+      <c r="A274" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B274" s="2" t="s">
@@ -7439,8 +7465,8 @@
         <v>549</v>
       </c>
     </row>
-    <row r="275" spans="1:4">
-      <c r="A275" s="2" t="s">
+    <row r="275" spans="1:4" ht="12.75">
+      <c r="A275" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B275" s="2" t="s">
@@ -7453,8 +7479,8 @@
         <v>551</v>
       </c>
     </row>
-    <row r="276" spans="1:4">
-      <c r="A276" s="4" t="s">
+    <row r="276" spans="1:4" ht="12.75">
+      <c r="A276" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B276" s="4" t="s">
@@ -7467,8 +7493,8 @@
         <v>553</v>
       </c>
     </row>
-    <row r="277" spans="1:4">
-      <c r="A277" s="4" t="s">
+    <row r="277" spans="1:4" ht="12.75">
+      <c r="A277" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B277" s="4" t="s">
@@ -7481,8 +7507,8 @@
         <v>555</v>
       </c>
     </row>
-    <row r="278" spans="1:4">
-      <c r="A278" s="2" t="s">
+    <row r="278" spans="1:4" ht="12.75">
+      <c r="A278" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B278" s="2" t="s">
@@ -7495,8 +7521,8 @@
         <v>557</v>
       </c>
     </row>
-    <row r="279" spans="1:4">
-      <c r="A279" s="4" t="s">
+    <row r="279" spans="1:4" ht="12.75">
+      <c r="A279" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B279" s="4" t="s">
@@ -7509,8 +7535,8 @@
         <v>559</v>
       </c>
     </row>
-    <row r="280" spans="1:4">
-      <c r="A280" s="4" t="s">
+    <row r="280" spans="1:4" ht="12.75">
+      <c r="A280" s="29" t="s">
         <v>533</v>
       </c>
       <c r="B280" s="4" t="s">
@@ -7523,8 +7549,8 @@
         <v>561</v>
       </c>
     </row>
-    <row r="281" spans="1:4">
-      <c r="A281" s="4" t="s">
+    <row r="281" spans="1:4" ht="12.75">
+      <c r="A281" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B281" s="4" t="s">
@@ -7537,8 +7563,8 @@
         <v>563</v>
       </c>
     </row>
-    <row r="282" spans="1:4">
-      <c r="A282" s="4" t="s">
+    <row r="282" spans="1:4" ht="12.75">
+      <c r="A282" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B282" s="4" t="s">
@@ -7551,8 +7577,8 @@
         <v>565</v>
       </c>
     </row>
-    <row r="283" spans="1:4">
-      <c r="A283" s="2" t="s">
+    <row r="283" spans="1:4" ht="12.75">
+      <c r="A283" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B283" s="2" t="s">
@@ -7565,8 +7591,8 @@
         <v>567</v>
       </c>
     </row>
-    <row r="284" spans="1:4">
-      <c r="A284" s="4" t="s">
+    <row r="284" spans="1:4" ht="12.75">
+      <c r="A284" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B284" s="4" t="s">
@@ -7579,8 +7605,8 @@
         <v>569</v>
       </c>
     </row>
-    <row r="285" spans="1:4">
-      <c r="A285" s="2" t="s">
+    <row r="285" spans="1:4" ht="12.75">
+      <c r="A285" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B285" s="2" t="s">
@@ -7593,8 +7619,8 @@
         <v>571</v>
       </c>
     </row>
-    <row r="286" spans="1:4">
-      <c r="A286" s="4" t="s">
+    <row r="286" spans="1:4" ht="12.75">
+      <c r="A286" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B286" s="4" t="s">
@@ -7607,8 +7633,8 @@
         <v>573</v>
       </c>
     </row>
-    <row r="287" spans="1:4">
-      <c r="A287" s="2" t="s">
+    <row r="287" spans="1:4" ht="12.75">
+      <c r="A287" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B287" s="2" t="s">
@@ -7621,8 +7647,8 @@
         <v>575</v>
       </c>
     </row>
-    <row r="288" spans="1:4">
-      <c r="A288" s="2" t="s">
+    <row r="288" spans="1:4" ht="12.75">
+      <c r="A288" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B288" s="2" t="s">
@@ -7635,8 +7661,8 @@
         <v>577</v>
       </c>
     </row>
-    <row r="289" spans="1:26">
-      <c r="A289" s="4" t="s">
+    <row r="289" spans="1:26" ht="12.75">
+      <c r="A289" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B289" s="4" t="s">
@@ -7649,8 +7675,8 @@
         <v>579</v>
       </c>
     </row>
-    <row r="290" spans="1:26">
-      <c r="A290" s="2" t="s">
+    <row r="290" spans="1:26" ht="12.75">
+      <c r="A290" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B290" s="2" t="s">
@@ -7663,8 +7689,8 @@
         <v>581</v>
       </c>
     </row>
-    <row r="291" spans="1:26">
-      <c r="A291" s="4" t="s">
+    <row r="291" spans="1:26" ht="12.75">
+      <c r="A291" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B291" s="4" t="s">
@@ -7677,8 +7703,8 @@
         <v>583</v>
       </c>
     </row>
-    <row r="292" spans="1:26">
-      <c r="A292" s="2" t="s">
+    <row r="292" spans="1:26" ht="12.75">
+      <c r="A292" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B292" s="2" t="s">
@@ -7691,8 +7717,8 @@
         <v>585</v>
       </c>
     </row>
-    <row r="293" spans="1:26">
-      <c r="A293" s="4" t="s">
+    <row r="293" spans="1:26" ht="12.75">
+      <c r="A293" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B293" s="4" t="s">
@@ -7705,8 +7731,8 @@
         <v>587</v>
       </c>
     </row>
-    <row r="294" spans="1:26">
-      <c r="A294" s="4" t="s">
+    <row r="294" spans="1:26" ht="12.75">
+      <c r="A294" s="29" t="s">
         <v>533</v>
       </c>
       <c r="B294" s="4" t="s">
@@ -7719,8 +7745,8 @@
         <v>589</v>
       </c>
     </row>
-    <row r="295" spans="1:26">
-      <c r="A295" s="4" t="s">
+    <row r="295" spans="1:26" ht="12.75">
+      <c r="A295" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B295" s="4" t="s">
@@ -7733,8 +7759,8 @@
         <v>591</v>
       </c>
     </row>
-    <row r="296" spans="1:26">
-      <c r="A296" s="2" t="s">
+    <row r="296" spans="1:26" ht="12.75">
+      <c r="A296" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B296" s="2" t="s">
@@ -7752,8 +7778,8 @@
       <c r="Y296" s="2"/>
       <c r="Z296" s="2"/>
     </row>
-    <row r="297" spans="1:26">
-      <c r="A297" s="4" t="s">
+    <row r="297" spans="1:26" ht="12.75">
+      <c r="A297" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B297" s="4" t="s">
@@ -7766,8 +7792,8 @@
         <v>595</v>
       </c>
     </row>
-    <row r="298" spans="1:26">
-      <c r="A298" s="4" t="s">
+    <row r="298" spans="1:26" ht="12.75">
+      <c r="A298" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B298" s="4" t="s">
@@ -7780,8 +7806,8 @@
         <v>597</v>
       </c>
     </row>
-    <row r="299" spans="1:26">
-      <c r="A299" s="4" t="s">
+    <row r="299" spans="1:26" ht="12.75">
+      <c r="A299" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B299" s="4" t="s">
@@ -7794,8 +7820,8 @@
         <v>599</v>
       </c>
     </row>
-    <row r="300" spans="1:26">
-      <c r="A300" s="4" t="s">
+    <row r="300" spans="1:26" ht="12.75">
+      <c r="A300" s="29" t="s">
         <v>533</v>
       </c>
       <c r="B300" s="4" t="s">
@@ -7808,8 +7834,8 @@
         <v>601</v>
       </c>
     </row>
-    <row r="301" spans="1:26">
-      <c r="A301" s="4" t="s">
+    <row r="301" spans="1:26" ht="12.75">
+      <c r="A301" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B301" s="4" t="s">
@@ -7822,8 +7848,8 @@
         <v>603</v>
       </c>
     </row>
-    <row r="302" spans="1:26">
-      <c r="A302" s="4" t="s">
+    <row r="302" spans="1:26" ht="12.75">
+      <c r="A302" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B302" s="4" t="s">
@@ -7836,8 +7862,8 @@
         <v>605</v>
       </c>
     </row>
-    <row r="303" spans="1:26">
-      <c r="A303" s="4" t="s">
+    <row r="303" spans="1:26" ht="12.75">
+      <c r="A303" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B303" s="4" t="s">
@@ -7850,8 +7876,8 @@
         <v>607</v>
       </c>
     </row>
-    <row r="304" spans="1:26">
-      <c r="A304" s="4" t="s">
+    <row r="304" spans="1:26" ht="12.75">
+      <c r="A304" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B304" s="4" t="s">
@@ -7864,8 +7890,8 @@
         <v>609</v>
       </c>
     </row>
-    <row r="305" spans="1:4">
-      <c r="A305" s="4" t="s">
+    <row r="305" spans="1:4" ht="12.75">
+      <c r="A305" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B305" s="4" t="s">
@@ -7878,8 +7904,8 @@
         <v>611</v>
       </c>
     </row>
-    <row r="306" spans="1:4">
-      <c r="A306" s="2" t="s">
+    <row r="306" spans="1:4" ht="12.75">
+      <c r="A306" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B306" s="9" t="s">
@@ -7892,8 +7918,8 @@
         <v>613</v>
       </c>
     </row>
-    <row r="307" spans="1:4">
-      <c r="A307" s="4" t="s">
+    <row r="307" spans="1:4" ht="12.75">
+      <c r="A307" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B307" s="4" t="s">
@@ -7906,8 +7932,8 @@
         <v>615</v>
       </c>
     </row>
-    <row r="308" spans="1:4">
-      <c r="A308" s="4" t="s">
+    <row r="308" spans="1:4" ht="12.75">
+      <c r="A308" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B308" s="4" t="s">
@@ -7920,8 +7946,8 @@
         <v>617</v>
       </c>
     </row>
-    <row r="309" spans="1:4">
-      <c r="A309" s="4" t="s">
+    <row r="309" spans="1:4" ht="12.75">
+      <c r="A309" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B309" s="4" t="s">
@@ -7934,8 +7960,8 @@
         <v>619</v>
       </c>
     </row>
-    <row r="310" spans="1:4">
-      <c r="A310" s="4" t="s">
+    <row r="310" spans="1:4" ht="12.75">
+      <c r="A310" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B310" s="4" t="s">
@@ -7948,8 +7974,8 @@
         <v>621</v>
       </c>
     </row>
-    <row r="311" spans="1:4">
-      <c r="A311" s="2" t="s">
+    <row r="311" spans="1:4" ht="12.75">
+      <c r="A311" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B311" s="2" t="s">
@@ -7962,8 +7988,8 @@
         <v>623</v>
       </c>
     </row>
-    <row r="312" spans="1:4">
-      <c r="A312" s="4" t="s">
+    <row r="312" spans="1:4" ht="12.75">
+      <c r="A312" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B312" s="4" t="s">
@@ -7976,8 +8002,8 @@
         <v>625</v>
       </c>
     </row>
-    <row r="313" spans="1:4">
-      <c r="A313" s="4" t="s">
+    <row r="313" spans="1:4" ht="12.75">
+      <c r="A313" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B313" s="4" t="s">
@@ -7990,8 +8016,8 @@
         <v>627</v>
       </c>
     </row>
-    <row r="314" spans="1:4">
-      <c r="A314" s="4" t="s">
+    <row r="314" spans="1:4" ht="12.75">
+      <c r="A314" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B314" s="4" t="s">
@@ -8004,8 +8030,8 @@
         <v>629</v>
       </c>
     </row>
-    <row r="315" spans="1:4">
-      <c r="A315" s="4" t="s">
+    <row r="315" spans="1:4" ht="12.75">
+      <c r="A315" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B315" s="5" t="s">
@@ -8018,8 +8044,8 @@
         <v>631</v>
       </c>
     </row>
-    <row r="316" spans="1:4">
-      <c r="A316" s="4" t="s">
+    <row r="316" spans="1:4" ht="12.75">
+      <c r="A316" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B316" s="4" t="s">
@@ -8032,8 +8058,8 @@
         <v>633</v>
       </c>
     </row>
-    <row r="317" spans="1:4">
-      <c r="A317" s="4" t="s">
+    <row r="317" spans="1:4" ht="12.75">
+      <c r="A317" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B317" s="4" t="s">
@@ -8046,8 +8072,8 @@
         <v>635</v>
       </c>
     </row>
-    <row r="318" spans="1:4">
-      <c r="A318" s="4" t="s">
+    <row r="318" spans="1:4" ht="12.75">
+      <c r="A318" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B318" s="4" t="s">
@@ -8060,8 +8086,8 @@
         <v>637</v>
       </c>
     </row>
-    <row r="319" spans="1:4">
-      <c r="A319" s="2" t="s">
+    <row r="319" spans="1:4" ht="12.75">
+      <c r="A319" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B319" s="2" t="s">
@@ -8074,8 +8100,8 @@
         <v>639</v>
       </c>
     </row>
-    <row r="320" spans="1:4">
-      <c r="A320" s="2" t="s">
+    <row r="320" spans="1:4" ht="12.75">
+      <c r="A320" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B320" s="2" t="s">
@@ -8088,8 +8114,8 @@
         <v>641</v>
       </c>
     </row>
-    <row r="321" spans="1:26">
-      <c r="A321" s="4" t="s">
+    <row r="321" spans="1:26" ht="12.75">
+      <c r="A321" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B321" s="4" t="s">
@@ -8102,8 +8128,8 @@
         <v>643</v>
       </c>
     </row>
-    <row r="322" spans="1:26">
-      <c r="A322" s="4" t="s">
+    <row r="322" spans="1:26" ht="12.75">
+      <c r="A322" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B322" s="4" t="s">
@@ -8116,8 +8142,8 @@
         <v>645</v>
       </c>
     </row>
-    <row r="323" spans="1:26">
-      <c r="A323" s="2" t="s">
+    <row r="323" spans="1:26" ht="12.75">
+      <c r="A323" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B323" s="2" t="s">
@@ -8130,8 +8156,8 @@
         <v>647</v>
       </c>
     </row>
-    <row r="324" spans="1:26">
-      <c r="A324" s="4" t="s">
+    <row r="324" spans="1:26" ht="12.75">
+      <c r="A324" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B324" s="4" t="s">
@@ -8144,8 +8170,8 @@
         <v>649</v>
       </c>
     </row>
-    <row r="325" spans="1:26">
-      <c r="A325" s="4" t="s">
+    <row r="325" spans="1:26" ht="12.75">
+      <c r="A325" s="29" t="s">
         <v>533</v>
       </c>
       <c r="B325" s="4" t="s">
@@ -8158,8 +8184,8 @@
         <v>651</v>
       </c>
     </row>
-    <row r="326" spans="1:26">
-      <c r="A326" s="4" t="s">
+    <row r="326" spans="1:26" ht="12.75">
+      <c r="A326" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B326" s="4" t="s">
@@ -8172,8 +8198,8 @@
         <v>653</v>
       </c>
     </row>
-    <row r="327" spans="1:26">
-      <c r="A327" s="4" t="s">
+    <row r="327" spans="1:26" ht="12.75">
+      <c r="A327" s="29" t="s">
         <v>533</v>
       </c>
       <c r="B327" s="4" t="s">
@@ -8186,8 +8212,8 @@
         <v>655</v>
       </c>
     </row>
-    <row r="328" spans="1:26">
-      <c r="A328" s="4" t="s">
+    <row r="328" spans="1:26" ht="12.75">
+      <c r="A328" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B328" s="4" t="s">
@@ -8200,8 +8226,8 @@
         <v>657</v>
       </c>
     </row>
-    <row r="329" spans="1:26">
-      <c r="A329" s="4" t="s">
+    <row r="329" spans="1:26" ht="12.75">
+      <c r="A329" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B329" s="4" t="s">
@@ -8214,8 +8240,8 @@
         <v>659</v>
       </c>
     </row>
-    <row r="330" spans="1:26">
-      <c r="A330" s="4" t="s">
+    <row r="330" spans="1:26" ht="12.75">
+      <c r="A330" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B330" s="4" t="s">
@@ -8228,8 +8254,8 @@
         <v>661</v>
       </c>
     </row>
-    <row r="331" spans="1:26">
-      <c r="A331" s="4" t="s">
+    <row r="331" spans="1:26" ht="12.75">
+      <c r="A331" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B331" s="4" t="s">
@@ -8242,8 +8268,8 @@
         <v>663</v>
       </c>
     </row>
-    <row r="332" spans="1:26">
-      <c r="A332" s="4" t="s">
+    <row r="332" spans="1:26" ht="12.75">
+      <c r="A332" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B332" s="4" t="s">
@@ -8256,8 +8282,8 @@
         <v>665</v>
       </c>
     </row>
-    <row r="333" spans="1:26">
-      <c r="A333" s="4" t="s">
+    <row r="333" spans="1:26" ht="12.75">
+      <c r="A333" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B333" s="4" t="s">
@@ -8275,8 +8301,8 @@
       <c r="Y333" s="2"/>
       <c r="Z333" s="2"/>
     </row>
-    <row r="334" spans="1:26">
-      <c r="A334" s="4" t="s">
+    <row r="334" spans="1:26" ht="12.75">
+      <c r="A334" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B334" s="4" t="s">
@@ -8289,8 +8315,8 @@
         <v>669</v>
       </c>
     </row>
-    <row r="335" spans="1:26">
-      <c r="A335" s="2" t="s">
+    <row r="335" spans="1:26" ht="12.75">
+      <c r="A335" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B335" s="2" t="s">
@@ -8303,8 +8329,8 @@
         <v>671</v>
       </c>
     </row>
-    <row r="336" spans="1:26">
-      <c r="A336" s="4" t="s">
+    <row r="336" spans="1:26" ht="12.75">
+      <c r="A336" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B336" s="4" t="s">
@@ -8317,8 +8343,8 @@
         <v>673</v>
       </c>
     </row>
-    <row r="337" spans="1:4">
-      <c r="A337" s="4" t="s">
+    <row r="337" spans="1:4" ht="12.75">
+      <c r="A337" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B337" s="4" t="s">
@@ -8331,8 +8357,8 @@
         <v>675</v>
       </c>
     </row>
-    <row r="338" spans="1:4">
-      <c r="A338" s="4" t="s">
+    <row r="338" spans="1:4" ht="12.75">
+      <c r="A338" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B338" s="4" t="s">
@@ -8345,8 +8371,8 @@
         <v>677</v>
       </c>
     </row>
-    <row r="339" spans="1:4">
-      <c r="A339" s="4" t="s">
+    <row r="339" spans="1:4" ht="12.75">
+      <c r="A339" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B339" s="4" t="s">
@@ -8359,8 +8385,8 @@
         <v>679</v>
       </c>
     </row>
-    <row r="340" spans="1:4">
-      <c r="A340" s="4" t="s">
+    <row r="340" spans="1:4" ht="12.75">
+      <c r="A340" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B340" s="4" t="s">
@@ -8373,8 +8399,8 @@
         <v>681</v>
       </c>
     </row>
-    <row r="341" spans="1:4">
-      <c r="A341" s="4" t="s">
+    <row r="341" spans="1:4" ht="12.75">
+      <c r="A341" s="29" t="s">
         <v>533</v>
       </c>
       <c r="B341" s="4" t="s">
@@ -8387,8 +8413,8 @@
         <v>683</v>
       </c>
     </row>
-    <row r="342" spans="1:4">
-      <c r="A342" s="4" t="s">
+    <row r="342" spans="1:4" ht="12.75">
+      <c r="A342" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B342" s="4" t="s">
@@ -8401,8 +8427,8 @@
         <v>685</v>
       </c>
     </row>
-    <row r="343" spans="1:4">
-      <c r="A343" s="4" t="s">
+    <row r="343" spans="1:4" ht="12.75">
+      <c r="A343" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B343" s="4" t="s">
@@ -8415,8 +8441,8 @@
         <v>687</v>
       </c>
     </row>
-    <row r="344" spans="1:4">
-      <c r="A344" s="2" t="s">
+    <row r="344" spans="1:4" ht="12.75">
+      <c r="A344" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B344" s="2" t="s">
@@ -8429,8 +8455,8 @@
         <v>689</v>
       </c>
     </row>
-    <row r="345" spans="1:4">
-      <c r="A345" s="2" t="s">
+    <row r="345" spans="1:4" ht="12.75">
+      <c r="A345" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B345" s="2" t="s">
@@ -8443,8 +8469,8 @@
         <v>691</v>
       </c>
     </row>
-    <row r="346" spans="1:4">
-      <c r="A346" s="4" t="s">
+    <row r="346" spans="1:4" ht="12.75">
+      <c r="A346" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B346" s="4" t="s">
@@ -8457,8 +8483,8 @@
         <v>693</v>
       </c>
     </row>
-    <row r="347" spans="1:4">
-      <c r="A347" s="4" t="s">
+    <row r="347" spans="1:4" ht="12.75">
+      <c r="A347" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B347" s="4" t="s">
@@ -8471,8 +8497,8 @@
         <v>695</v>
       </c>
     </row>
-    <row r="348" spans="1:4">
-      <c r="A348" s="4" t="s">
+    <row r="348" spans="1:4" ht="12.75">
+      <c r="A348" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B348" s="4" t="s">
@@ -8485,8 +8511,8 @@
         <v>697</v>
       </c>
     </row>
-    <row r="349" spans="1:4">
-      <c r="A349" s="4" t="s">
+    <row r="349" spans="1:4" ht="12.75">
+      <c r="A349" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B349" s="4" t="s">
@@ -8499,8 +8525,8 @@
         <v>699</v>
       </c>
     </row>
-    <row r="350" spans="1:4">
-      <c r="A350" s="4" t="s">
+    <row r="350" spans="1:4" ht="12.75">
+      <c r="A350" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B350" s="4" t="s">
@@ -8513,8 +8539,8 @@
         <v>701</v>
       </c>
     </row>
-    <row r="351" spans="1:4">
-      <c r="A351" s="4" t="s">
+    <row r="351" spans="1:4" ht="12.75">
+      <c r="A351" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B351" s="4" t="s">
@@ -8527,8 +8553,8 @@
         <v>703</v>
       </c>
     </row>
-    <row r="352" spans="1:4">
-      <c r="A352" s="2" t="s">
+    <row r="352" spans="1:4" ht="12.75">
+      <c r="A352" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B352" s="2" t="s">
@@ -8541,8 +8567,8 @@
         <v>705</v>
       </c>
     </row>
-    <row r="353" spans="1:4">
-      <c r="A353" s="2" t="s">
+    <row r="353" spans="1:4" ht="12.75">
+      <c r="A353" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B353" s="2" t="s">
@@ -8555,8 +8581,8 @@
         <v>707</v>
       </c>
     </row>
-    <row r="354" spans="1:4">
-      <c r="A354" s="2" t="s">
+    <row r="354" spans="1:4" ht="12.75">
+      <c r="A354" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B354" s="3" t="s">
@@ -8569,8 +8595,8 @@
         <v>709</v>
       </c>
     </row>
-    <row r="355" spans="1:4">
-      <c r="A355" s="4" t="s">
+    <row r="355" spans="1:4" ht="12.75">
+      <c r="A355" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B355" s="4" t="s">
@@ -8583,8 +8609,8 @@
         <v>711</v>
       </c>
     </row>
-    <row r="356" spans="1:4">
-      <c r="A356" s="2" t="s">
+    <row r="356" spans="1:4" ht="12.75">
+      <c r="A356" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B356" s="2" t="s">
@@ -8597,8 +8623,8 @@
         <v>713</v>
       </c>
     </row>
-    <row r="357" spans="1:4">
-      <c r="A357" s="2" t="s">
+    <row r="357" spans="1:4" ht="12.75">
+      <c r="A357" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B357" s="3" t="s">
@@ -8611,8 +8637,8 @@
         <v>715</v>
       </c>
     </row>
-    <row r="358" spans="1:4">
-      <c r="A358" s="4" t="s">
+    <row r="358" spans="1:4" ht="12.75">
+      <c r="A358" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B358" s="4" t="s">
@@ -8625,8 +8651,8 @@
         <v>717</v>
       </c>
     </row>
-    <row r="359" spans="1:4">
-      <c r="A359" s="4" t="s">
+    <row r="359" spans="1:4" ht="12.75">
+      <c r="A359" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B359" s="4" t="s">
@@ -8639,8 +8665,8 @@
         <v>719</v>
       </c>
     </row>
-    <row r="360" spans="1:4">
-      <c r="A360" s="4" t="s">
+    <row r="360" spans="1:4" ht="12.75">
+      <c r="A360" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B360" s="4" t="s">
@@ -8653,8 +8679,8 @@
         <v>721</v>
       </c>
     </row>
-    <row r="361" spans="1:4">
-      <c r="A361" s="4" t="s">
+    <row r="361" spans="1:4" ht="12.75">
+      <c r="A361" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B361" s="4" t="s">
@@ -8667,8 +8693,8 @@
         <v>723</v>
       </c>
     </row>
-    <row r="362" spans="1:4">
-      <c r="A362" s="4" t="s">
+    <row r="362" spans="1:4" ht="12.75">
+      <c r="A362" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B362" s="4" t="s">
@@ -8681,8 +8707,8 @@
         <v>725</v>
       </c>
     </row>
-    <row r="363" spans="1:4">
-      <c r="A363" s="4" t="s">
+    <row r="363" spans="1:4" ht="12.75">
+      <c r="A363" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B363" s="4" t="s">
@@ -8695,8 +8721,8 @@
         <v>727</v>
       </c>
     </row>
-    <row r="364" spans="1:4">
-      <c r="A364" s="2" t="s">
+    <row r="364" spans="1:4" ht="12.75">
+      <c r="A364" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B364" s="2" t="s">
@@ -8709,8 +8735,8 @@
         <v>729</v>
       </c>
     </row>
-    <row r="365" spans="1:4">
-      <c r="A365" s="2" t="s">
+    <row r="365" spans="1:4" ht="12.75">
+      <c r="A365" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B365" s="2" t="s">
@@ -8723,8 +8749,8 @@
         <v>731</v>
       </c>
     </row>
-    <row r="366" spans="1:4">
-      <c r="A366" s="4" t="s">
+    <row r="366" spans="1:4" ht="12.75">
+      <c r="A366" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B366" s="4" t="s">
@@ -8737,8 +8763,8 @@
         <v>733</v>
       </c>
     </row>
-    <row r="367" spans="1:4">
-      <c r="A367" s="4" t="s">
+    <row r="367" spans="1:4" ht="12.75">
+      <c r="A367" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B367" s="4" t="s">
@@ -8751,8 +8777,8 @@
         <v>735</v>
       </c>
     </row>
-    <row r="368" spans="1:4">
-      <c r="A368" s="4" t="s">
+    <row r="368" spans="1:4" ht="12.75">
+      <c r="A368" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B368" s="4" t="s">
@@ -8765,8 +8791,8 @@
         <v>737</v>
       </c>
     </row>
-    <row r="369" spans="1:4">
-      <c r="A369" s="2" t="s">
+    <row r="369" spans="1:4" ht="12.75">
+      <c r="A369" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B369" s="2" t="s">
@@ -8779,8 +8805,8 @@
         <v>739</v>
       </c>
     </row>
-    <row r="370" spans="1:4">
-      <c r="A370" s="4" t="s">
+    <row r="370" spans="1:4" ht="12.75">
+      <c r="A370" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B370" s="4" t="s">
@@ -8793,8 +8819,8 @@
         <v>741</v>
       </c>
     </row>
-    <row r="371" spans="1:4">
-      <c r="A371" s="4" t="s">
+    <row r="371" spans="1:4" ht="12.75">
+      <c r="A371" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B371" s="4" t="s">
@@ -8807,8 +8833,8 @@
         <v>743</v>
       </c>
     </row>
-    <row r="372" spans="1:4">
-      <c r="A372" s="4" t="s">
+    <row r="372" spans="1:4" ht="12.75">
+      <c r="A372" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B372" s="4" t="s">
@@ -8821,8 +8847,8 @@
         <v>745</v>
       </c>
     </row>
-    <row r="373" spans="1:4">
-      <c r="A373" s="4" t="s">
+    <row r="373" spans="1:4" ht="12.75">
+      <c r="A373" s="29" t="s">
         <v>530</v>
       </c>
       <c r="B373" s="4" t="s">
@@ -8835,8 +8861,8 @@
         <v>747</v>
       </c>
     </row>
-    <row r="374" spans="1:4">
-      <c r="A374" s="4" t="s">
+    <row r="374" spans="1:4" ht="12.75">
+      <c r="A374" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B374" s="4" t="s">
@@ -8849,8 +8875,8 @@
         <v>750</v>
       </c>
     </row>
-    <row r="375" spans="1:4">
-      <c r="A375" s="2" t="s">
+    <row r="375" spans="1:4" ht="12.75">
+      <c r="A375" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B375" s="2" t="s">
@@ -8863,8 +8889,8 @@
         <v>752</v>
       </c>
     </row>
-    <row r="376" spans="1:4">
-      <c r="A376" s="2" t="s">
+    <row r="376" spans="1:4" ht="12.75">
+      <c r="A376" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B376" s="2" t="s">
@@ -8877,8 +8903,8 @@
         <v>754</v>
       </c>
     </row>
-    <row r="377" spans="1:4">
-      <c r="A377" s="2" t="s">
+    <row r="377" spans="1:4" ht="12.75">
+      <c r="A377" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B377" s="2" t="s">
@@ -8891,8 +8917,8 @@
         <v>756</v>
       </c>
     </row>
-    <row r="378" spans="1:4">
-      <c r="A378" s="4" t="s">
+    <row r="378" spans="1:4" ht="12.75">
+      <c r="A378" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B378" s="4" t="s">
@@ -8905,8 +8931,8 @@
         <v>758</v>
       </c>
     </row>
-    <row r="379" spans="1:4">
-      <c r="A379" s="4" t="s">
+    <row r="379" spans="1:4" ht="12.75">
+      <c r="A379" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B379" s="4" t="s">
@@ -8919,8 +8945,8 @@
         <v>760</v>
       </c>
     </row>
-    <row r="380" spans="1:4">
-      <c r="A380" s="2" t="s">
+    <row r="380" spans="1:4" ht="12.75">
+      <c r="A380" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B380" s="2" t="s">
@@ -8933,8 +8959,8 @@
         <v>762</v>
       </c>
     </row>
-    <row r="381" spans="1:4">
-      <c r="A381" s="2" t="s">
+    <row r="381" spans="1:4" ht="12.75">
+      <c r="A381" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B381" s="2" t="s">
@@ -8947,8 +8973,8 @@
         <v>764</v>
       </c>
     </row>
-    <row r="382" spans="1:4">
-      <c r="A382" s="2" t="s">
+    <row r="382" spans="1:4" ht="12.75">
+      <c r="A382" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B382" s="9" t="s">
@@ -8961,8 +8987,8 @@
         <v>766</v>
       </c>
     </row>
-    <row r="383" spans="1:4">
-      <c r="A383" s="4" t="s">
+    <row r="383" spans="1:4" ht="12.75">
+      <c r="A383" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B383" s="10" t="s">
@@ -8975,8 +9001,8 @@
         <v>768</v>
       </c>
     </row>
-    <row r="384" spans="1:4">
-      <c r="A384" s="4" t="s">
+    <row r="384" spans="1:4" ht="12.75">
+      <c r="A384" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B384" s="10" t="s">
@@ -8989,8 +9015,8 @@
         <v>770</v>
       </c>
     </row>
-    <row r="385" spans="1:4">
-      <c r="A385" s="4" t="s">
+    <row r="385" spans="1:4" ht="12.75">
+      <c r="A385" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B385" s="10" t="s">
@@ -9003,8 +9029,8 @@
         <v>772</v>
       </c>
     </row>
-    <row r="386" spans="1:4">
-      <c r="A386" s="4" t="s">
+    <row r="386" spans="1:4" ht="12.75">
+      <c r="A386" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B386" s="10" t="s">
@@ -9017,8 +9043,8 @@
         <v>774</v>
       </c>
     </row>
-    <row r="387" spans="1:4">
-      <c r="A387" s="4" t="s">
+    <row r="387" spans="1:4" ht="12.75">
+      <c r="A387" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B387" s="10" t="s">
@@ -9031,8 +9057,8 @@
         <v>776</v>
       </c>
     </row>
-    <row r="388" spans="1:4">
-      <c r="A388" s="4" t="s">
+    <row r="388" spans="1:4" ht="12.75">
+      <c r="A388" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B388" s="10" t="s">
@@ -9045,8 +9071,8 @@
         <v>778</v>
       </c>
     </row>
-    <row r="389" spans="1:4">
-      <c r="A389" s="4" t="s">
+    <row r="389" spans="1:4" ht="12.75">
+      <c r="A389" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B389" s="10" t="s">
@@ -9059,8 +9085,8 @@
         <v>780</v>
       </c>
     </row>
-    <row r="390" spans="1:4">
-      <c r="A390" s="2" t="s">
+    <row r="390" spans="1:4" ht="12.75">
+      <c r="A390" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B390" s="9" t="s">
@@ -9073,8 +9099,8 @@
         <v>782</v>
       </c>
     </row>
-    <row r="391" spans="1:4">
-      <c r="A391" s="4" t="s">
+    <row r="391" spans="1:4" ht="12.75">
+      <c r="A391" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B391" s="10" t="s">
@@ -9087,8 +9113,8 @@
         <v>784</v>
       </c>
     </row>
-    <row r="392" spans="1:4">
-      <c r="A392" s="4" t="s">
+    <row r="392" spans="1:4" ht="12.75">
+      <c r="A392" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B392" s="10" t="s">
@@ -9101,8 +9127,8 @@
         <v>786</v>
       </c>
     </row>
-    <row r="393" spans="1:4">
-      <c r="A393" s="4" t="s">
+    <row r="393" spans="1:4" ht="12.75">
+      <c r="A393" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B393" s="10" t="s">
@@ -9115,8 +9141,8 @@
         <v>788</v>
       </c>
     </row>
-    <row r="394" spans="1:4">
-      <c r="A394" s="4" t="s">
+    <row r="394" spans="1:4" ht="12.75">
+      <c r="A394" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B394" s="10" t="s">
@@ -9129,8 +9155,8 @@
         <v>790</v>
       </c>
     </row>
-    <row r="395" spans="1:4">
-      <c r="A395" s="4" t="s">
+    <row r="395" spans="1:4" ht="12.75">
+      <c r="A395" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B395" s="10" t="s">
@@ -9143,8 +9169,8 @@
         <v>792</v>
       </c>
     </row>
-    <row r="396" spans="1:4">
-      <c r="A396" s="4" t="s">
+    <row r="396" spans="1:4" ht="12.75">
+      <c r="A396" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B396" s="10" t="s">
@@ -9157,8 +9183,8 @@
         <v>794</v>
       </c>
     </row>
-    <row r="397" spans="1:4">
-      <c r="A397" s="4" t="s">
+    <row r="397" spans="1:4" ht="12.75">
+      <c r="A397" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B397" s="10" t="s">
@@ -9171,8 +9197,8 @@
         <v>796</v>
       </c>
     </row>
-    <row r="398" spans="1:4">
-      <c r="A398" s="4" t="s">
+    <row r="398" spans="1:4" ht="12.75">
+      <c r="A398" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B398" s="10" t="s">
@@ -9185,8 +9211,8 @@
         <v>798</v>
       </c>
     </row>
-    <row r="399" spans="1:4">
-      <c r="A399" s="2" t="s">
+    <row r="399" spans="1:4" ht="12.75">
+      <c r="A399" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B399" s="9" t="s">
@@ -9199,8 +9225,8 @@
         <v>800</v>
       </c>
     </row>
-    <row r="400" spans="1:4">
-      <c r="A400" s="4" t="s">
+    <row r="400" spans="1:4" ht="12.75">
+      <c r="A400" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B400" s="10" t="s">
@@ -9213,8 +9239,8 @@
         <v>802</v>
       </c>
     </row>
-    <row r="401" spans="1:26">
-      <c r="A401" s="4" t="s">
+    <row r="401" spans="1:26" ht="12.75">
+      <c r="A401" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B401" s="10" t="s">
@@ -9227,8 +9253,8 @@
         <v>804</v>
       </c>
     </row>
-    <row r="402" spans="1:26">
-      <c r="A402" s="2" t="s">
+    <row r="402" spans="1:26" ht="12.75">
+      <c r="A402" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B402" s="9" t="s">
@@ -9241,8 +9267,8 @@
         <v>806</v>
       </c>
     </row>
-    <row r="403" spans="1:26">
-      <c r="A403" s="24" t="s">
+    <row r="403" spans="1:26" ht="12.75">
+      <c r="A403" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B403" s="24" t="s">
@@ -9277,8 +9303,8 @@
       <c r="Y403" s="6"/>
       <c r="Z403" s="6"/>
     </row>
-    <row r="404" spans="1:26">
-      <c r="A404" s="4" t="s">
+    <row r="404" spans="1:26" ht="12.75">
+      <c r="A404" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B404" s="4" t="s">
@@ -9291,8 +9317,8 @@
         <v>810</v>
       </c>
     </row>
-    <row r="405" spans="1:26">
-      <c r="A405" s="2" t="s">
+    <row r="405" spans="1:26" ht="12.75">
+      <c r="A405" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B405" s="2" t="s">
@@ -9305,8 +9331,8 @@
         <v>812</v>
       </c>
     </row>
-    <row r="406" spans="1:26">
-      <c r="A406" s="2" t="s">
+    <row r="406" spans="1:26" ht="12.75">
+      <c r="A406" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B406" s="2" t="s">
@@ -9319,8 +9345,8 @@
         <v>814</v>
       </c>
     </row>
-    <row r="407" spans="1:26">
-      <c r="A407" s="4" t="s">
+    <row r="407" spans="1:26" ht="12.75">
+      <c r="A407" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B407" s="4" t="s">
@@ -9333,8 +9359,8 @@
         <v>816</v>
       </c>
     </row>
-    <row r="408" spans="1:26">
-      <c r="A408" s="4" t="s">
+    <row r="408" spans="1:26" ht="12.75">
+      <c r="A408" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B408" s="4" t="s">
@@ -9347,8 +9373,8 @@
         <v>818</v>
       </c>
     </row>
-    <row r="409" spans="1:26">
-      <c r="A409" s="2" t="s">
+    <row r="409" spans="1:26" ht="12.75">
+      <c r="A409" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B409" s="2" t="s">
@@ -9361,8 +9387,8 @@
         <v>820</v>
       </c>
     </row>
-    <row r="410" spans="1:26">
-      <c r="A410" s="4" t="s">
+    <row r="410" spans="1:26" ht="12.75">
+      <c r="A410" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B410" s="4" t="s">
@@ -9375,8 +9401,8 @@
         <v>822</v>
       </c>
     </row>
-    <row r="411" spans="1:26">
-      <c r="A411" s="4" t="s">
+    <row r="411" spans="1:26" ht="12.75">
+      <c r="A411" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B411" s="4" t="s">
@@ -9389,8 +9415,8 @@
         <v>824</v>
       </c>
     </row>
-    <row r="412" spans="1:26">
-      <c r="A412" s="2" t="s">
+    <row r="412" spans="1:26" ht="12.75">
+      <c r="A412" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B412" s="2" t="s">
@@ -9403,8 +9429,8 @@
         <v>826</v>
       </c>
     </row>
-    <row r="413" spans="1:26">
-      <c r="A413" s="2" t="s">
+    <row r="413" spans="1:26" ht="12.75">
+      <c r="A413" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B413" s="2" t="s">
@@ -9417,8 +9443,8 @@
         <v>828</v>
       </c>
     </row>
-    <row r="414" spans="1:26">
-      <c r="A414" s="4" t="s">
+    <row r="414" spans="1:26" ht="12.75">
+      <c r="A414" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B414" s="4" t="s">
@@ -9431,8 +9457,8 @@
         <v>830</v>
       </c>
     </row>
-    <row r="415" spans="1:26">
-      <c r="A415" s="2" t="s">
+    <row r="415" spans="1:26" ht="12.75">
+      <c r="A415" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B415" s="2" t="s">
@@ -9445,8 +9471,8 @@
         <v>832</v>
       </c>
     </row>
-    <row r="416" spans="1:26">
-      <c r="A416" s="4" t="s">
+    <row r="416" spans="1:26" ht="12.75">
+      <c r="A416" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B416" s="4" t="s">
@@ -9459,8 +9485,8 @@
         <v>834</v>
       </c>
     </row>
-    <row r="417" spans="1:4">
-      <c r="A417" s="2" t="s">
+    <row r="417" spans="1:4" ht="12.75">
+      <c r="A417" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B417" s="2" t="s">
@@ -9473,8 +9499,8 @@
         <v>836</v>
       </c>
     </row>
-    <row r="418" spans="1:4">
-      <c r="A418" s="2" t="s">
+    <row r="418" spans="1:4" ht="12.75">
+      <c r="A418" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B418" s="2" t="s">
@@ -9487,8 +9513,8 @@
         <v>838</v>
       </c>
     </row>
-    <row r="419" spans="1:4">
-      <c r="A419" s="2" t="s">
+    <row r="419" spans="1:4" ht="12.75">
+      <c r="A419" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B419" s="2" t="s">
@@ -9501,8 +9527,8 @@
         <v>840</v>
       </c>
     </row>
-    <row r="420" spans="1:4">
-      <c r="A420" s="2" t="s">
+    <row r="420" spans="1:4" ht="12.75">
+      <c r="A420" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B420" s="2" t="s">
@@ -9515,8 +9541,8 @@
         <v>842</v>
       </c>
     </row>
-    <row r="421" spans="1:4">
-      <c r="A421" s="4" t="s">
+    <row r="421" spans="1:4" ht="12.75">
+      <c r="A421" s="29" t="s">
         <v>748</v>
       </c>
       <c r="B421" s="4" t="s">
@@ -9529,8 +9555,8 @@
         <v>844</v>
       </c>
     </row>
-    <row r="422" spans="1:4">
-      <c r="A422" s="2" t="s">
+    <row r="422" spans="1:4" ht="12.75">
+      <c r="A422" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B422" s="2" t="s">
@@ -9543,8 +9569,8 @@
         <v>846</v>
       </c>
     </row>
-    <row r="423" spans="1:4">
-      <c r="A423" s="2" t="s">
+    <row r="423" spans="1:4" ht="12.75">
+      <c r="A423" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B423" s="2" t="s">

</xml_diff>

<commit_message>
Added code and analysis for lifetime reproductive fitness fig
</commit_message>
<xml_diff>
--- a/potentially_eligible_papers.xlsx
+++ b/potentially_eligible_papers.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9C844B-4385-43F8-9365-4BD054849870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C01902-30DC-4BEC-A537-C0BAD5E93DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scan 1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>BOX PLOTS
@@ -697,6 +698,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Hosken</t>
     </r>
@@ -705,6 +707,7 @@
         <sz val="10"/>
         <color rgb="FF1F1F1F"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> et al. </t>
     </r>
@@ -713,6 +716,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(2003)</t>
     </r>
@@ -3179,54 +3183,64 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3337,7 +3351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3381,17 +3395,15 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3617,20 +3629,20 @@
   </sheetPr>
   <dimension ref="A1:Z423"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A386" workbookViewId="0">
-      <selection activeCell="C400" sqref="C400"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="37.7109375" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" customWidth="1"/>
     <col min="4" max="4" width="96.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="12.75">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3644,7 +3656,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3658,7 +3670,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -3672,7 +3684,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3686,7 +3698,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -3700,7 +3712,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -3714,7 +3726,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -3728,7 +3740,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -3742,7 +3754,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3756,7 +3768,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -3770,7 +3782,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3784,7 +3796,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -3798,7 +3810,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -3812,7 +3824,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -3826,7 +3838,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3840,7 +3852,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -3854,7 +3866,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="12.75">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -3868,7 +3880,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="12.75">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -3882,7 +3894,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="12.75">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -3896,7 +3908,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="12.75">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -3910,7 +3922,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -3924,7 +3936,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.75">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -3938,7 +3950,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="12.75">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -3952,7 +3964,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="12.75">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -3966,7 +3978,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="12.75">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -3980,7 +3992,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="12.75">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -3994,7 +4006,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="12.75">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -4008,7 +4020,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="12.75">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -4022,7 +4034,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="12.75">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -4036,7 +4048,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="12.75">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -4050,7 +4062,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="12.75">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -4064,7 +4076,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="12.75">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -4078,7 +4090,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="12.75">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -4092,7 +4104,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="12.75">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -4106,7 +4118,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="12.75">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -4120,7 +4132,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="12.75">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -4134,7 +4146,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -4148,7 +4160,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="12.75">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -4162,7 +4174,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -4176,7 +4188,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -4190,7 +4202,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -4204,7 +4216,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -4218,7 +4230,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -4232,7 +4244,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="12.75">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -4246,7 +4258,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="12.75">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -4260,7 +4272,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="12.75">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -4274,7 +4286,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -4288,7 +4300,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -4302,7 +4314,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -4316,7 +4328,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75">
-      <c r="A50" s="28" t="s">
+      <c r="A50" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -4330,7 +4342,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="12.75">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -4344,7 +4356,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -4358,7 +4370,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -4372,7 +4384,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -4386,7 +4398,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -4400,7 +4412,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -4414,7 +4426,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75">
-      <c r="A57" s="29" t="s">
+      <c r="A57" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -4428,7 +4440,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="12.75">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -4442,7 +4454,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75">
-      <c r="A59" s="28" t="s">
+      <c r="A59" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -4456,7 +4468,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -4470,7 +4482,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75">
-      <c r="A61" s="29" t="s">
+      <c r="A61" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -4484,7 +4496,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75">
-      <c r="A62" s="29" t="s">
+      <c r="A62" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -4498,7 +4510,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -4512,7 +4524,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75">
-      <c r="A64" s="28" t="s">
+      <c r="A64" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -4526,7 +4538,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75">
-      <c r="A65" s="29" t="s">
+      <c r="A65" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -4540,7 +4552,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75">
-      <c r="A66" s="28" t="s">
+      <c r="A66" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -4554,7 +4566,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75">
-      <c r="A67" s="29" t="s">
+      <c r="A67" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -4568,7 +4580,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75">
-      <c r="A68" s="28" t="s">
+      <c r="A68" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -4582,7 +4594,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75">
-      <c r="A69" s="29" t="s">
+      <c r="A69" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -4596,7 +4608,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75">
-      <c r="A70" s="29" t="s">
+      <c r="A70" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -4610,7 +4622,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75">
-      <c r="A71" s="29" t="s">
+      <c r="A71" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B71" s="4" t="s">
@@ -4624,7 +4636,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="12.75">
-      <c r="A72" s="29" t="s">
+      <c r="A72" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B72" s="4" t="s">
@@ -4638,7 +4650,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75">
-      <c r="A73" s="28" t="s">
+      <c r="A73" s="27" t="s">
         <v>1014</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -4652,7 +4664,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75">
-      <c r="A74" s="28" t="s">
+      <c r="A74" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B74" s="2" t="s">
@@ -4666,7 +4678,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75">
-      <c r="A75" s="28" t="s">
+      <c r="A75" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -4680,7 +4692,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75">
-      <c r="A76" s="28" t="s">
+      <c r="A76" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -4694,7 +4706,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75">
-      <c r="A77" s="28" t="s">
+      <c r="A77" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -4708,7 +4720,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75">
-      <c r="A78" s="28" t="s">
+      <c r="A78" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -4722,7 +4734,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="12.75">
-      <c r="A79" s="29" t="s">
+      <c r="A79" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B79" s="4" t="s">
@@ -4736,7 +4748,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75">
-      <c r="A80" s="29" t="s">
+      <c r="A80" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B80" s="4" t="s">
@@ -4750,7 +4762,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="12.75">
-      <c r="A81" s="29" t="s">
+      <c r="A81" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B81" s="4" t="s">
@@ -4764,7 +4776,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="12.75">
-      <c r="A82" s="29" t="s">
+      <c r="A82" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B82" s="4" t="s">
@@ -4778,7 +4790,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="12.75">
-      <c r="A83" s="30" t="s">
+      <c r="A83" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B83" s="4" t="s">
@@ -4792,7 +4804,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="12.75">
-      <c r="A84" s="29" t="s">
+      <c r="A84" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B84" s="4" t="s">
@@ -4806,7 +4818,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="12.75">
-      <c r="A85" s="29" t="s">
+      <c r="A85" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B85" s="4" t="s">
@@ -4820,7 +4832,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="12.75">
-      <c r="A86" s="28" t="s">
+      <c r="A86" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B86" s="2" t="s">
@@ -4834,7 +4846,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="12.75">
-      <c r="A87" s="29" t="s">
+      <c r="A87" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B87" s="4" t="s">
@@ -4848,7 +4860,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="12.75">
-      <c r="A88" s="28" t="s">
+      <c r="A88" s="27" t="s">
         <v>1014</v>
       </c>
       <c r="B88" s="2" t="s">
@@ -4862,7 +4874,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75">
-      <c r="A89" s="29" t="s">
+      <c r="A89" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B89" s="4" t="s">
@@ -4876,7 +4888,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="12.75">
-      <c r="A90" s="28" t="s">
+      <c r="A90" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B90" s="2" t="s">
@@ -4890,7 +4902,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="12.75">
-      <c r="A91" s="29" t="s">
+      <c r="A91" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B91" s="4" t="s">
@@ -4904,7 +4916,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="12.75">
-      <c r="A92" s="28" t="s">
+      <c r="A92" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B92" s="2" t="s">
@@ -4918,7 +4930,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="12.75">
-      <c r="A93" s="28" t="s">
+      <c r="A93" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B93" s="2" t="s">
@@ -4932,7 +4944,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="12.75">
-      <c r="A94" s="28" t="s">
+      <c r="A94" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B94" s="2" t="s">
@@ -4946,7 +4958,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="12.75">
-      <c r="A95" s="28" t="s">
+      <c r="A95" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B95" s="2" t="s">
@@ -4960,7 +4972,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="12.75">
-      <c r="A96" s="28" t="s">
+      <c r="A96" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B96" s="2" t="s">
@@ -4974,7 +4986,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="12.75">
-      <c r="A97" s="28" t="s">
+      <c r="A97" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -4988,7 +5000,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="12.75">
-      <c r="A98" s="29" t="s">
+      <c r="A98" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B98" s="4" t="s">
@@ -5002,7 +5014,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="12.75">
-      <c r="A99" s="29" t="s">
+      <c r="A99" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B99" s="4" t="s">
@@ -5016,7 +5028,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="12.75">
-      <c r="A100" s="28" t="s">
+      <c r="A100" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B100" s="2" t="s">
@@ -5030,7 +5042,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="12.75">
-      <c r="A101" s="28" t="s">
+      <c r="A101" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -5044,7 +5056,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="12.75">
-      <c r="A102" s="28" t="s">
+      <c r="A102" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="2" t="s">
@@ -5058,7 +5070,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="12.75">
-      <c r="A103" s="29" t="s">
+      <c r="A103" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B103" s="5" t="s">
@@ -5072,7 +5084,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="12.75">
-      <c r="A104" s="28" t="s">
+      <c r="A104" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B104" s="2" t="s">
@@ -5086,7 +5098,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" ht="12.75">
-      <c r="A105" s="28" t="s">
+      <c r="A105" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B105" s="2" t="s">
@@ -5100,7 +5112,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="12.75">
-      <c r="A106" s="29" t="s">
+      <c r="A106" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B106" s="4" t="s">
@@ -5114,7 +5126,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="12.75">
-      <c r="A107" s="28" t="s">
+      <c r="A107" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B107" s="2" t="s">
@@ -5128,7 +5140,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" ht="12.75">
-      <c r="A108" s="28" t="s">
+      <c r="A108" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B108" s="2" t="s">
@@ -5142,7 +5154,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="12.75">
-      <c r="A109" s="28" t="s">
+      <c r="A109" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -5156,7 +5168,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="12.75">
-      <c r="A110" s="28" t="s">
+      <c r="A110" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B110" s="2" t="s">
@@ -5170,7 +5182,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="12.75">
-      <c r="A111" s="29" t="s">
+      <c r="A111" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B111" s="4" t="s">
@@ -5184,7 +5196,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="12.75">
-      <c r="A112" s="30" t="s">
+      <c r="A112" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B112" s="4" t="s">
@@ -5198,7 +5210,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="12.75">
-      <c r="A113" s="28" t="s">
+      <c r="A113" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B113" s="2" t="s">
@@ -5212,7 +5224,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="12.75">
-      <c r="A114" s="28" t="s">
+      <c r="A114" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B114" s="2" t="s">
@@ -5226,7 +5238,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" ht="12.75">
-      <c r="A115" s="29" t="s">
+      <c r="A115" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B115" s="4" t="s">
@@ -5240,7 +5252,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" ht="12.75">
-      <c r="A116" s="29" t="s">
+      <c r="A116" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B116" s="4" t="s">
@@ -5254,7 +5266,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" ht="12.75">
-      <c r="A117" s="29" t="s">
+      <c r="A117" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B117" s="4" t="s">
@@ -5268,7 +5280,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="12.75">
-      <c r="A118" s="28" t="s">
+      <c r="A118" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B118" s="2" t="s">
@@ -5282,7 +5294,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" ht="12.75">
-      <c r="A119" s="28" t="s">
+      <c r="A119" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B119" s="2" t="s">
@@ -5296,7 +5308,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" ht="12.75">
-      <c r="A120" s="28" t="s">
+      <c r="A120" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B120" s="2" t="s">
@@ -5310,7 +5322,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" ht="12.75">
-      <c r="A121" s="28" t="s">
+      <c r="A121" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B121" s="2" t="s">
@@ -5324,7 +5336,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" ht="12.75">
-      <c r="A122" s="29" t="s">
+      <c r="A122" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B122" s="4" t="s">
@@ -5338,7 +5350,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" ht="12.75">
-      <c r="A123" s="28" t="s">
+      <c r="A123" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B123" s="2" t="s">
@@ -5352,7 +5364,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" ht="12.75">
-      <c r="A124" s="28" t="s">
+      <c r="A124" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B124" s="2" t="s">
@@ -5366,7 +5378,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" ht="12.75">
-      <c r="A125" s="29" t="s">
+      <c r="A125" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B125" s="4" t="s">
@@ -5380,7 +5392,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" ht="12.75">
-      <c r="A126" s="28" t="s">
+      <c r="A126" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B126" s="2" t="s">
@@ -5394,7 +5406,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="12.75">
-      <c r="A127" s="28" t="s">
+      <c r="A127" s="27" t="s">
         <v>1014</v>
       </c>
       <c r="B127" s="2" t="s">
@@ -5408,7 +5420,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" ht="12.75">
-      <c r="A128" s="29" t="s">
+      <c r="A128" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B128" s="4" t="s">
@@ -5422,7 +5434,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" ht="12.75">
-      <c r="A129" s="29" t="s">
+      <c r="A129" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B129" s="4" t="s">
@@ -5436,7 +5448,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" ht="12.75">
-      <c r="A130" s="28" t="s">
+      <c r="A130" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B130" s="2" t="s">
@@ -5450,7 +5462,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" ht="12.75">
-      <c r="A131" s="28" t="s">
+      <c r="A131" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B131" s="2" t="s">
@@ -5464,7 +5476,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="12.75">
-      <c r="A132" s="28" t="s">
+      <c r="A132" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B132" s="2" t="s">
@@ -5478,7 +5490,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" ht="12.75">
-      <c r="A133" s="29" t="s">
+      <c r="A133" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B133" s="4" t="s">
@@ -5492,7 +5504,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" ht="12.75">
-      <c r="A134" s="28" t="s">
+      <c r="A134" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B134" s="2" t="s">
@@ -5506,7 +5518,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" ht="12.75">
-      <c r="A135" s="29" t="s">
+      <c r="A135" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B135" s="4" t="s">
@@ -5520,7 +5532,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" ht="12.75">
-      <c r="A136" s="29" t="s">
+      <c r="A136" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B136" s="4" t="s">
@@ -5534,7 +5546,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" ht="12.75">
-      <c r="A137" s="29" t="s">
+      <c r="A137" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B137" s="4" t="s">
@@ -5548,7 +5560,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" ht="12.75">
-      <c r="A138" s="28" t="s">
+      <c r="A138" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B138" s="2" t="s">
@@ -5562,7 +5574,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" ht="12.75">
-      <c r="A139" s="29" t="s">
+      <c r="A139" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B139" s="4" t="s">
@@ -5576,7 +5588,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" ht="12.75">
-      <c r="A140" s="28" t="s">
+      <c r="A140" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B140" s="2" t="s">
@@ -5590,7 +5602,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="12.75">
-      <c r="A141" s="28" t="s">
+      <c r="A141" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B141" s="2" t="s">
@@ -5604,7 +5616,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" ht="12.75">
-      <c r="A142" s="28" t="s">
+      <c r="A142" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B142" s="2" t="s">
@@ -5618,7 +5630,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" ht="12.75">
-      <c r="A143" s="28" t="s">
+      <c r="A143" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B143" s="2" t="s">
@@ -5632,7 +5644,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" ht="12.75">
-      <c r="A144" s="29" t="s">
+      <c r="A144" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B144" s="4" t="s">
@@ -5646,7 +5658,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="12.75">
-      <c r="A145" s="28" t="s">
+      <c r="A145" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B145" s="2" t="s">
@@ -5660,7 +5672,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="12.75">
-      <c r="A146" s="28" t="s">
+      <c r="A146" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B146" s="2" t="s">
@@ -5674,7 +5686,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" ht="12.75">
-      <c r="A147" s="29" t="s">
+      <c r="A147" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B147" s="4" t="s">
@@ -5688,7 +5700,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="12.75">
-      <c r="A148" s="29" t="s">
+      <c r="A148" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B148" s="4" t="s">
@@ -5702,7 +5714,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="12.75">
-      <c r="A149" s="28" t="s">
+      <c r="A149" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B149" s="2" t="s">
@@ -5716,7 +5728,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="12.75">
-      <c r="A150" s="28" t="s">
+      <c r="A150" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B150" s="2" t="s">
@@ -5730,7 +5742,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" ht="12.75">
-      <c r="A151" s="28" t="s">
+      <c r="A151" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B151" s="2" t="s">
@@ -5744,7 +5756,7 @@
       </c>
     </row>
     <row r="152" spans="1:4" ht="12.75">
-      <c r="A152" s="29" t="s">
+      <c r="A152" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B152" s="4" t="s">
@@ -5758,7 +5770,7 @@
       </c>
     </row>
     <row r="153" spans="1:4" ht="12.75">
-      <c r="A153" s="28" t="s">
+      <c r="A153" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B153" s="2" t="s">
@@ -5772,7 +5784,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="12.75">
-      <c r="A154" s="29" t="s">
+      <c r="A154" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B154" s="4" t="s">
@@ -5786,7 +5798,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" ht="12.75">
-      <c r="A155" s="29" t="s">
+      <c r="A155" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B155" s="4" t="s">
@@ -5800,7 +5812,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" ht="12.75">
-      <c r="A156" s="28" t="s">
+      <c r="A156" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B156" s="2" t="s">
@@ -5814,7 +5826,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" ht="12.75">
-      <c r="A157" s="29" t="s">
+      <c r="A157" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B157" s="4" t="s">
@@ -5828,7 +5840,7 @@
       </c>
     </row>
     <row r="158" spans="1:4" ht="12.75">
-      <c r="A158" s="28" t="s">
+      <c r="A158" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B158" s="2" t="s">
@@ -5842,7 +5854,7 @@
       </c>
     </row>
     <row r="159" spans="1:4" ht="12.75">
-      <c r="A159" s="29" t="s">
+      <c r="A159" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B159" s="4" t="s">
@@ -5856,7 +5868,7 @@
       </c>
     </row>
     <row r="160" spans="1:4" ht="12.75">
-      <c r="A160" s="28" t="s">
+      <c r="A160" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B160" s="2" t="s">
@@ -5870,7 +5882,7 @@
       </c>
     </row>
     <row r="161" spans="1:4" ht="12.75">
-      <c r="A161" s="28" t="s">
+      <c r="A161" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B161" s="2" t="s">
@@ -5884,7 +5896,7 @@
       </c>
     </row>
     <row r="162" spans="1:4" ht="12.75">
-      <c r="A162" s="29" t="s">
+      <c r="A162" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B162" s="4" t="s">
@@ -5898,7 +5910,7 @@
       </c>
     </row>
     <row r="163" spans="1:4" ht="12.75">
-      <c r="A163" s="29" t="s">
+      <c r="A163" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B163" s="4" t="s">
@@ -5912,7 +5924,7 @@
       </c>
     </row>
     <row r="164" spans="1:4" ht="12.75">
-      <c r="A164" s="28" t="s">
+      <c r="A164" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B164" s="2" t="s">
@@ -5926,7 +5938,7 @@
       </c>
     </row>
     <row r="165" spans="1:4" ht="12.75">
-      <c r="A165" s="29" t="s">
+      <c r="A165" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B165" s="4" t="s">
@@ -5940,7 +5952,7 @@
       </c>
     </row>
     <row r="166" spans="1:4" ht="12.75">
-      <c r="A166" s="28" t="s">
+      <c r="A166" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B166" s="2" t="s">
@@ -5954,7 +5966,7 @@
       </c>
     </row>
     <row r="167" spans="1:4" ht="12.75">
-      <c r="A167" s="29" t="s">
+      <c r="A167" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B167" s="4" t="s">
@@ -5968,7 +5980,7 @@
       </c>
     </row>
     <row r="168" spans="1:4" ht="12.75">
-      <c r="A168" s="29" t="s">
+      <c r="A168" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B168" s="4" t="s">
@@ -5982,7 +5994,7 @@
       </c>
     </row>
     <row r="169" spans="1:4" ht="12.75">
-      <c r="A169" s="29" t="s">
+      <c r="A169" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B169" s="4" t="s">
@@ -5996,7 +6008,7 @@
       </c>
     </row>
     <row r="170" spans="1:4" ht="12.75">
-      <c r="A170" s="29" t="s">
+      <c r="A170" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B170" s="4" t="s">
@@ -6010,7 +6022,7 @@
       </c>
     </row>
     <row r="171" spans="1:4" ht="12.75">
-      <c r="A171" s="29" t="s">
+      <c r="A171" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B171" s="4" t="s">
@@ -6024,7 +6036,7 @@
       </c>
     </row>
     <row r="172" spans="1:4" ht="12.75">
-      <c r="A172" s="28" t="s">
+      <c r="A172" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B172" s="2" t="s">
@@ -6038,7 +6050,7 @@
       </c>
     </row>
     <row r="173" spans="1:4" ht="12.75">
-      <c r="A173" s="29" t="s">
+      <c r="A173" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B173" s="4" t="s">
@@ -6052,7 +6064,7 @@
       </c>
     </row>
     <row r="174" spans="1:4" ht="12.75">
-      <c r="A174" s="29" t="s">
+      <c r="A174" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B174" s="4" t="s">
@@ -6066,7 +6078,7 @@
       </c>
     </row>
     <row r="175" spans="1:4" ht="12.75">
-      <c r="A175" s="29" t="s">
+      <c r="A175" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B175" s="4" t="s">
@@ -6080,7 +6092,7 @@
       </c>
     </row>
     <row r="176" spans="1:4" ht="12.75">
-      <c r="A176" s="29" t="s">
+      <c r="A176" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B176" s="4" t="s">
@@ -6094,7 +6106,7 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="12.75">
-      <c r="A177" s="28" t="s">
+      <c r="A177" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B177" s="2" t="s">
@@ -6108,7 +6120,7 @@
       </c>
     </row>
     <row r="178" spans="1:4" ht="12.75">
-      <c r="A178" s="28" t="s">
+      <c r="A178" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B178" s="2" t="s">
@@ -6122,7 +6134,7 @@
       </c>
     </row>
     <row r="179" spans="1:4" ht="12.75">
-      <c r="A179" s="29" t="s">
+      <c r="A179" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B179" s="4" t="s">
@@ -6136,7 +6148,7 @@
       </c>
     </row>
     <row r="180" spans="1:4" ht="12.75">
-      <c r="A180" s="29" t="s">
+      <c r="A180" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B180" s="4" t="s">
@@ -6150,7 +6162,7 @@
       </c>
     </row>
     <row r="181" spans="1:4" ht="12.75">
-      <c r="A181" s="29" t="s">
+      <c r="A181" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B181" s="4" t="s">
@@ -6164,7 +6176,7 @@
       </c>
     </row>
     <row r="182" spans="1:4" ht="12.75">
-      <c r="A182" s="29" t="s">
+      <c r="A182" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B182" s="4" t="s">
@@ -6178,7 +6190,7 @@
       </c>
     </row>
     <row r="183" spans="1:4" ht="12.75">
-      <c r="A183" s="29" t="s">
+      <c r="A183" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B183" s="5" t="s">
@@ -6192,7 +6204,7 @@
       </c>
     </row>
     <row r="184" spans="1:4" ht="12.75">
-      <c r="A184" s="29" t="s">
+      <c r="A184" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B184" s="4" t="s">
@@ -6206,7 +6218,7 @@
       </c>
     </row>
     <row r="185" spans="1:4" ht="12.75">
-      <c r="A185" s="28" t="s">
+      <c r="A185" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B185" s="2" t="s">
@@ -6220,7 +6232,7 @@
       </c>
     </row>
     <row r="186" spans="1:4" ht="12.75">
-      <c r="A186" s="29" t="s">
+      <c r="A186" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B186" s="4" t="s">
@@ -6234,7 +6246,7 @@
       </c>
     </row>
     <row r="187" spans="1:4" ht="12.75">
-      <c r="A187" s="29" t="s">
+      <c r="A187" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B187" s="4" t="s">
@@ -6248,7 +6260,7 @@
       </c>
     </row>
     <row r="188" spans="1:4" ht="12.75">
-      <c r="A188" s="28" t="s">
+      <c r="A188" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B188" s="2" t="s">
@@ -6262,7 +6274,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" ht="12.75">
-      <c r="A189" s="29" t="s">
+      <c r="A189" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B189" s="4" t="s">
@@ -6276,7 +6288,7 @@
       </c>
     </row>
     <row r="190" spans="1:4" ht="12.75">
-      <c r="A190" s="29" t="s">
+      <c r="A190" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B190" s="4" t="s">
@@ -6290,7 +6302,7 @@
       </c>
     </row>
     <row r="191" spans="1:4" ht="12.75">
-      <c r="A191" s="28" t="s">
+      <c r="A191" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B191" s="2" t="s">
@@ -6304,7 +6316,7 @@
       </c>
     </row>
     <row r="192" spans="1:4" ht="12.75">
-      <c r="A192" s="28" t="s">
+      <c r="A192" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B192" s="2" t="s">
@@ -6318,7 +6330,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" ht="12.75">
-      <c r="A193" s="28" t="s">
+      <c r="A193" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B193" s="2" t="s">
@@ -6332,7 +6344,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" ht="12.75">
-      <c r="A194" s="29" t="s">
+      <c r="A194" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B194" s="4" t="s">
@@ -6346,7 +6358,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" ht="12.75">
-      <c r="A195" s="28" t="s">
+      <c r="A195" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B195" s="2" t="s">
@@ -6360,7 +6372,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" ht="12.75">
-      <c r="A196" s="29" t="s">
+      <c r="A196" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B196" s="4" t="s">
@@ -6374,7 +6386,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" ht="12.75">
-      <c r="A197" s="28" t="s">
+      <c r="A197" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B197" s="2" t="s">
@@ -6388,7 +6400,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" ht="12.75">
-      <c r="A198" s="29" t="s">
+      <c r="A198" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B198" s="4" t="s">
@@ -6402,7 +6414,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" ht="12.75">
-      <c r="A199" s="29" t="s">
+      <c r="A199" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B199" s="4" t="s">
@@ -6416,7 +6428,7 @@
       </c>
     </row>
     <row r="200" spans="1:4" ht="12.75">
-      <c r="A200" s="28" t="s">
+      <c r="A200" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B200" s="2" t="s">
@@ -6430,7 +6442,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" ht="12.75">
-      <c r="A201" s="29" t="s">
+      <c r="A201" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B201" s="4" t="s">
@@ -6444,7 +6456,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" ht="12.75">
-      <c r="A202" s="29" t="s">
+      <c r="A202" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B202" s="4" t="s">
@@ -6458,7 +6470,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" ht="12.75">
-      <c r="A203" s="28" t="s">
+      <c r="A203" s="27" t="s">
         <v>1014</v>
       </c>
       <c r="B203" s="2" t="s">
@@ -6472,7 +6484,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" ht="12.75">
-      <c r="A204" s="29" t="s">
+      <c r="A204" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B204" s="4" t="s">
@@ -6486,7 +6498,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" ht="12.75">
-      <c r="A205" s="29" t="s">
+      <c r="A205" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B205" s="4" t="s">
@@ -6500,7 +6512,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" ht="12.75">
-      <c r="A206" s="29" t="s">
+      <c r="A206" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B206" s="4" t="s">
@@ -6514,7 +6526,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" ht="12.75">
-      <c r="A207" s="29" t="s">
+      <c r="A207" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B207" s="4" t="s">
@@ -6528,7 +6540,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" ht="12.75">
-      <c r="A208" s="29" t="s">
+      <c r="A208" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B208" s="4" t="s">
@@ -6542,7 +6554,7 @@
       </c>
     </row>
     <row r="209" spans="1:4" ht="12.75">
-      <c r="A209" s="29" t="s">
+      <c r="A209" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B209" s="4" t="s">
@@ -6556,7 +6568,7 @@
       </c>
     </row>
     <row r="210" spans="1:4" ht="12.75">
-      <c r="A210" s="29" t="s">
+      <c r="A210" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B210" s="4" t="s">
@@ -6570,7 +6582,7 @@
       </c>
     </row>
     <row r="211" spans="1:4" ht="12.75">
-      <c r="A211" s="29" t="s">
+      <c r="A211" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B211" s="4" t="s">
@@ -6584,7 +6596,7 @@
       </c>
     </row>
     <row r="212" spans="1:4" ht="12.75">
-      <c r="A212" s="28" t="s">
+      <c r="A212" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B212" s="2" t="s">
@@ -6598,7 +6610,7 @@
       </c>
     </row>
     <row r="213" spans="1:4" ht="12.75">
-      <c r="A213" s="29" t="s">
+      <c r="A213" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B213" s="4" t="s">
@@ -6612,7 +6624,7 @@
       </c>
     </row>
     <row r="214" spans="1:4" ht="12.75">
-      <c r="A214" s="29" t="s">
+      <c r="A214" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B214" s="4" t="s">
@@ -6626,7 +6638,7 @@
       </c>
     </row>
     <row r="215" spans="1:4" ht="12.75">
-      <c r="A215" s="29" t="s">
+      <c r="A215" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B215" s="4" t="s">
@@ -6640,7 +6652,7 @@
       </c>
     </row>
     <row r="216" spans="1:4" ht="12.75">
-      <c r="A216" s="29" t="s">
+      <c r="A216" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B216" s="4" t="s">
@@ -6654,7 +6666,7 @@
       </c>
     </row>
     <row r="217" spans="1:4" ht="12.75">
-      <c r="A217" s="29" t="s">
+      <c r="A217" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B217" s="4" t="s">
@@ -6668,7 +6680,7 @@
       </c>
     </row>
     <row r="218" spans="1:4" ht="12.75">
-      <c r="A218" s="30" t="s">
+      <c r="A218" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B218" s="4" t="s">
@@ -6682,7 +6694,7 @@
       </c>
     </row>
     <row r="219" spans="1:4" ht="12.75">
-      <c r="A219" s="28" t="s">
+      <c r="A219" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B219" s="2" t="s">
@@ -6696,7 +6708,7 @@
       </c>
     </row>
     <row r="220" spans="1:4" ht="12.75">
-      <c r="A220" s="28" t="s">
+      <c r="A220" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B220" s="2" t="s">
@@ -6710,7 +6722,7 @@
       </c>
     </row>
     <row r="221" spans="1:4" ht="12.75">
-      <c r="A221" s="29" t="s">
+      <c r="A221" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B221" s="4" t="s">
@@ -6724,7 +6736,7 @@
       </c>
     </row>
     <row r="222" spans="1:4" ht="12.75">
-      <c r="A222" s="29" t="s">
+      <c r="A222" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B222" s="4" t="s">
@@ -6738,7 +6750,7 @@
       </c>
     </row>
     <row r="223" spans="1:4" ht="12.75">
-      <c r="A223" s="28" t="s">
+      <c r="A223" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B223" s="2" t="s">
@@ -6752,7 +6764,7 @@
       </c>
     </row>
     <row r="224" spans="1:4" ht="12.75">
-      <c r="A224" s="29" t="s">
+      <c r="A224" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B224" s="4" t="s">
@@ -6766,7 +6778,7 @@
       </c>
     </row>
     <row r="225" spans="1:4" ht="12.75">
-      <c r="A225" s="29" t="s">
+      <c r="A225" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B225" s="4" t="s">
@@ -6780,7 +6792,7 @@
       </c>
     </row>
     <row r="226" spans="1:4" ht="12.75">
-      <c r="A226" s="29" t="s">
+      <c r="A226" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B226" s="4" t="s">
@@ -6794,7 +6806,7 @@
       </c>
     </row>
     <row r="227" spans="1:4" ht="12.75">
-      <c r="A227" s="29" t="s">
+      <c r="A227" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B227" s="4" t="s">
@@ -6808,7 +6820,7 @@
       </c>
     </row>
     <row r="228" spans="1:4" ht="12.75">
-      <c r="A228" s="28" t="s">
+      <c r="A228" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B228" s="2" t="s">
@@ -6822,7 +6834,7 @@
       </c>
     </row>
     <row r="229" spans="1:4" ht="12.75">
-      <c r="A229" s="29" t="s">
+      <c r="A229" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B229" s="4" t="s">
@@ -6836,7 +6848,7 @@
       </c>
     </row>
     <row r="230" spans="1:4" ht="12.75">
-      <c r="A230" s="28" t="s">
+      <c r="A230" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B230" s="2" t="s">
@@ -6850,7 +6862,7 @@
       </c>
     </row>
     <row r="231" spans="1:4" ht="12.75">
-      <c r="A231" s="29" t="s">
+      <c r="A231" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B231" s="4" t="s">
@@ -6864,7 +6876,7 @@
       </c>
     </row>
     <row r="232" spans="1:4" ht="12.75">
-      <c r="A232" s="28" t="s">
+      <c r="A232" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B232" s="2" t="s">
@@ -6878,7 +6890,7 @@
       </c>
     </row>
     <row r="233" spans="1:4" ht="12.75">
-      <c r="A233" s="28" t="s">
+      <c r="A233" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B233" s="2" t="s">
@@ -6892,7 +6904,7 @@
       </c>
     </row>
     <row r="234" spans="1:4" ht="12.75">
-      <c r="A234" s="28" t="s">
+      <c r="A234" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B234" s="4" t="s">
@@ -6906,7 +6918,7 @@
       </c>
     </row>
     <row r="235" spans="1:4" ht="12.75">
-      <c r="A235" s="29" t="s">
+      <c r="A235" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B235" s="4" t="s">
@@ -6920,7 +6932,7 @@
       </c>
     </row>
     <row r="236" spans="1:4" ht="12.75">
-      <c r="A236" s="29" t="s">
+      <c r="A236" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B236" s="4" t="s">
@@ -6934,7 +6946,7 @@
       </c>
     </row>
     <row r="237" spans="1:4" ht="12.75">
-      <c r="A237" s="29" t="s">
+      <c r="A237" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B237" s="4" t="s">
@@ -6948,7 +6960,7 @@
       </c>
     </row>
     <row r="238" spans="1:4" ht="12.75">
-      <c r="A238" s="29" t="s">
+      <c r="A238" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B238" s="4" t="s">
@@ -6962,7 +6974,7 @@
       </c>
     </row>
     <row r="239" spans="1:4" ht="12.75">
-      <c r="A239" s="28" t="s">
+      <c r="A239" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B239" s="2" t="s">
@@ -6976,7 +6988,7 @@
       </c>
     </row>
     <row r="240" spans="1:4" ht="12.75">
-      <c r="A240" s="28" t="s">
+      <c r="A240" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B240" s="2" t="s">
@@ -6990,7 +7002,7 @@
       </c>
     </row>
     <row r="241" spans="1:4" ht="12.75">
-      <c r="A241" s="29" t="s">
+      <c r="A241" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B241" s="4" t="s">
@@ -7004,7 +7016,7 @@
       </c>
     </row>
     <row r="242" spans="1:4" ht="12.75">
-      <c r="A242" s="29" t="s">
+      <c r="A242" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B242" s="4" t="s">
@@ -7018,7 +7030,7 @@
       </c>
     </row>
     <row r="243" spans="1:4" ht="12.75">
-      <c r="A243" s="29" t="s">
+      <c r="A243" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B243" s="4" t="s">
@@ -7032,7 +7044,7 @@
       </c>
     </row>
     <row r="244" spans="1:4" ht="12.75">
-      <c r="A244" s="29" t="s">
+      <c r="A244" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B244" s="4" t="s">
@@ -7046,7 +7058,7 @@
       </c>
     </row>
     <row r="245" spans="1:4" ht="12.75">
-      <c r="A245" s="29" t="s">
+      <c r="A245" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B245" s="4" t="s">
@@ -7060,7 +7072,7 @@
       </c>
     </row>
     <row r="246" spans="1:4" ht="12.75">
-      <c r="A246" s="28" t="s">
+      <c r="A246" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B246" s="2" t="s">
@@ -7074,7 +7086,7 @@
       </c>
     </row>
     <row r="247" spans="1:4" ht="12.75">
-      <c r="A247" s="29" t="s">
+      <c r="A247" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B247" s="4" t="s">
@@ -7088,7 +7100,7 @@
       </c>
     </row>
     <row r="248" spans="1:4" ht="12.75">
-      <c r="A248" s="28" t="s">
+      <c r="A248" s="27" t="s">
         <v>1014</v>
       </c>
       <c r="B248" s="2" t="s">
@@ -7102,7 +7114,7 @@
       </c>
     </row>
     <row r="249" spans="1:4" ht="12.75">
-      <c r="A249" s="29" t="s">
+      <c r="A249" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B249" s="4" t="s">
@@ -7116,7 +7128,7 @@
       </c>
     </row>
     <row r="250" spans="1:4" ht="12.75">
-      <c r="A250" s="28" t="s">
+      <c r="A250" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
@@ -7130,7 +7142,7 @@
       </c>
     </row>
     <row r="251" spans="1:4" ht="12.75">
-      <c r="A251" s="28" t="s">
+      <c r="A251" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B251" s="2" t="s">
@@ -7144,7 +7156,7 @@
       </c>
     </row>
     <row r="252" spans="1:4" ht="12.75">
-      <c r="A252" s="29" t="s">
+      <c r="A252" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B252" s="4" t="s">
@@ -7158,7 +7170,7 @@
       </c>
     </row>
     <row r="253" spans="1:4" ht="12.75">
-      <c r="A253" s="29" t="s">
+      <c r="A253" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B253" s="4" t="s">
@@ -7172,7 +7184,7 @@
       </c>
     </row>
     <row r="254" spans="1:4" ht="12.75">
-      <c r="A254" s="29" t="s">
+      <c r="A254" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B254" s="4" t="s">
@@ -7186,7 +7198,7 @@
       </c>
     </row>
     <row r="255" spans="1:4" ht="12.75">
-      <c r="A255" s="28" t="s">
+      <c r="A255" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B255" s="2" t="s">
@@ -7200,7 +7212,7 @@
       </c>
     </row>
     <row r="256" spans="1:4" ht="12.75">
-      <c r="A256" s="29" t="s">
+      <c r="A256" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B256" s="4" t="s">
@@ -7214,7 +7226,7 @@
       </c>
     </row>
     <row r="257" spans="1:4" ht="12.75">
-      <c r="A257" s="28" t="s">
+      <c r="A257" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B257" s="2" t="s">
@@ -7228,7 +7240,7 @@
       </c>
     </row>
     <row r="258" spans="1:4" ht="12.75">
-      <c r="A258" s="29" t="s">
+      <c r="A258" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B258" s="4" t="s">
@@ -7242,7 +7254,7 @@
       </c>
     </row>
     <row r="259" spans="1:4" ht="12.75">
-      <c r="A259" s="29" t="s">
+      <c r="A259" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B259" s="4" t="s">
@@ -7256,7 +7268,7 @@
       </c>
     </row>
     <row r="260" spans="1:4" ht="12.75">
-      <c r="A260" s="29" t="s">
+      <c r="A260" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B260" s="4" t="s">
@@ -7270,7 +7282,7 @@
       </c>
     </row>
     <row r="261" spans="1:4" ht="12.75">
-      <c r="A261" s="29" t="s">
+      <c r="A261" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B261" s="4" t="s">
@@ -7284,7 +7296,7 @@
       </c>
     </row>
     <row r="262" spans="1:4" ht="12.75">
-      <c r="A262" s="29" t="s">
+      <c r="A262" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B262" s="4" t="s">
@@ -7298,7 +7310,7 @@
       </c>
     </row>
     <row r="263" spans="1:4" ht="12.75">
-      <c r="A263" s="29" t="s">
+      <c r="A263" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B263" s="4" t="s">
@@ -7312,7 +7324,7 @@
       </c>
     </row>
     <row r="264" spans="1:4" ht="12.75">
-      <c r="A264" s="29" t="s">
+      <c r="A264" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B264" s="4" t="s">
@@ -7326,7 +7338,7 @@
       </c>
     </row>
     <row r="265" spans="1:4" ht="12.75">
-      <c r="A265" s="29" t="s">
+      <c r="A265" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B265" s="4" t="s">
@@ -7340,7 +7352,7 @@
       </c>
     </row>
     <row r="266" spans="1:4" ht="12.75">
-      <c r="A266" s="28" t="s">
+      <c r="A266" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B266" s="2" t="s">
@@ -7354,7 +7366,7 @@
       </c>
     </row>
     <row r="267" spans="1:4" ht="12.75">
-      <c r="A267" s="28" t="s">
+      <c r="A267" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B267" s="2" t="s">
@@ -7368,7 +7380,7 @@
       </c>
     </row>
     <row r="268" spans="1:4" ht="12.75">
-      <c r="A268" s="29" t="s">
+      <c r="A268" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B268" s="4" t="s">
@@ -7382,7 +7394,7 @@
       </c>
     </row>
     <row r="269" spans="1:4" ht="12.75">
-      <c r="A269" s="28" t="s">
+      <c r="A269" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B269" s="2" t="s">
@@ -7396,7 +7408,7 @@
       </c>
     </row>
     <row r="270" spans="1:4" ht="12.75">
-      <c r="A270" s="29" t="s">
+      <c r="A270" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B270" s="7" t="s">
@@ -7410,7 +7422,7 @@
       </c>
     </row>
     <row r="271" spans="1:4" ht="12.75">
-      <c r="A271" s="28" t="s">
+      <c r="A271" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B271" s="8" t="s">
@@ -7424,7 +7436,7 @@
       </c>
     </row>
     <row r="272" spans="1:4" ht="12.75">
-      <c r="A272" s="28" t="s">
+      <c r="A272" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B272" s="8" t="s">
@@ -7438,7 +7450,7 @@
       </c>
     </row>
     <row r="273" spans="1:4" ht="12.75">
-      <c r="A273" s="29" t="s">
+      <c r="A273" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B273" s="5" t="s">
@@ -7452,7 +7464,7 @@
       </c>
     </row>
     <row r="274" spans="1:4" ht="12.75">
-      <c r="A274" s="28" t="s">
+      <c r="A274" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B274" s="2" t="s">
@@ -7466,7 +7478,7 @@
       </c>
     </row>
     <row r="275" spans="1:4" ht="12.75">
-      <c r="A275" s="28" t="s">
+      <c r="A275" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B275" s="2" t="s">
@@ -7480,7 +7492,7 @@
       </c>
     </row>
     <row r="276" spans="1:4" ht="12.75">
-      <c r="A276" s="29" t="s">
+      <c r="A276" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B276" s="4" t="s">
@@ -7494,7 +7506,7 @@
       </c>
     </row>
     <row r="277" spans="1:4" ht="12.75">
-      <c r="A277" s="29" t="s">
+      <c r="A277" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B277" s="4" t="s">
@@ -7508,7 +7520,7 @@
       </c>
     </row>
     <row r="278" spans="1:4" ht="12.75">
-      <c r="A278" s="28" t="s">
+      <c r="A278" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B278" s="2" t="s">
@@ -7522,7 +7534,7 @@
       </c>
     </row>
     <row r="279" spans="1:4" ht="12.75">
-      <c r="A279" s="29" t="s">
+      <c r="A279" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B279" s="4" t="s">
@@ -7536,7 +7548,7 @@
       </c>
     </row>
     <row r="280" spans="1:4" ht="12.75">
-      <c r="A280" s="29" t="s">
+      <c r="A280" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B280" s="4" t="s">
@@ -7550,7 +7562,7 @@
       </c>
     </row>
     <row r="281" spans="1:4" ht="12.75">
-      <c r="A281" s="29" t="s">
+      <c r="A281" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B281" s="4" t="s">
@@ -7564,7 +7576,7 @@
       </c>
     </row>
     <row r="282" spans="1:4" ht="12.75">
-      <c r="A282" s="29" t="s">
+      <c r="A282" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B282" s="4" t="s">
@@ -7578,7 +7590,7 @@
       </c>
     </row>
     <row r="283" spans="1:4" ht="12.75">
-      <c r="A283" s="28" t="s">
+      <c r="A283" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B283" s="2" t="s">
@@ -7592,7 +7604,7 @@
       </c>
     </row>
     <row r="284" spans="1:4" ht="12.75">
-      <c r="A284" s="29" t="s">
+      <c r="A284" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B284" s="4" t="s">
@@ -7606,7 +7618,7 @@
       </c>
     </row>
     <row r="285" spans="1:4" ht="12.75">
-      <c r="A285" s="28" t="s">
+      <c r="A285" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B285" s="2" t="s">
@@ -7620,7 +7632,7 @@
       </c>
     </row>
     <row r="286" spans="1:4" ht="12.75">
-      <c r="A286" s="29" t="s">
+      <c r="A286" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B286" s="4" t="s">
@@ -7634,7 +7646,7 @@
       </c>
     </row>
     <row r="287" spans="1:4" ht="12.75">
-      <c r="A287" s="28" t="s">
+      <c r="A287" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B287" s="2" t="s">
@@ -7648,7 +7660,7 @@
       </c>
     </row>
     <row r="288" spans="1:4" ht="12.75">
-      <c r="A288" s="28" t="s">
+      <c r="A288" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B288" s="2" t="s">
@@ -7662,7 +7674,7 @@
       </c>
     </row>
     <row r="289" spans="1:26" ht="12.75">
-      <c r="A289" s="29" t="s">
+      <c r="A289" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B289" s="4" t="s">
@@ -7676,7 +7688,7 @@
       </c>
     </row>
     <row r="290" spans="1:26" ht="12.75">
-      <c r="A290" s="28" t="s">
+      <c r="A290" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B290" s="2" t="s">
@@ -7690,7 +7702,7 @@
       </c>
     </row>
     <row r="291" spans="1:26" ht="12.75">
-      <c r="A291" s="29" t="s">
+      <c r="A291" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B291" s="4" t="s">
@@ -7704,7 +7716,7 @@
       </c>
     </row>
     <row r="292" spans="1:26" ht="12.75">
-      <c r="A292" s="28" t="s">
+      <c r="A292" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B292" s="2" t="s">
@@ -7718,7 +7730,7 @@
       </c>
     </row>
     <row r="293" spans="1:26" ht="12.75">
-      <c r="A293" s="29" t="s">
+      <c r="A293" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B293" s="4" t="s">
@@ -7732,7 +7744,7 @@
       </c>
     </row>
     <row r="294" spans="1:26" ht="12.75">
-      <c r="A294" s="29" t="s">
+      <c r="A294" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B294" s="4" t="s">
@@ -7746,7 +7758,7 @@
       </c>
     </row>
     <row r="295" spans="1:26" ht="12.75">
-      <c r="A295" s="29" t="s">
+      <c r="A295" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B295" s="4" t="s">
@@ -7760,7 +7772,7 @@
       </c>
     </row>
     <row r="296" spans="1:26" ht="12.75">
-      <c r="A296" s="28" t="s">
+      <c r="A296" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B296" s="2" t="s">
@@ -7779,7 +7791,7 @@
       <c r="Z296" s="2"/>
     </row>
     <row r="297" spans="1:26" ht="12.75">
-      <c r="A297" s="29" t="s">
+      <c r="A297" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B297" s="4" t="s">
@@ -7793,7 +7805,7 @@
       </c>
     </row>
     <row r="298" spans="1:26" ht="12.75">
-      <c r="A298" s="29" t="s">
+      <c r="A298" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B298" s="4" t="s">
@@ -7807,7 +7819,7 @@
       </c>
     </row>
     <row r="299" spans="1:26" ht="12.75">
-      <c r="A299" s="29" t="s">
+      <c r="A299" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B299" s="4" t="s">
@@ -7821,7 +7833,7 @@
       </c>
     </row>
     <row r="300" spans="1:26" ht="12.75">
-      <c r="A300" s="29" t="s">
+      <c r="A300" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B300" s="4" t="s">
@@ -7835,7 +7847,7 @@
       </c>
     </row>
     <row r="301" spans="1:26" ht="12.75">
-      <c r="A301" s="29" t="s">
+      <c r="A301" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B301" s="4" t="s">
@@ -7849,7 +7861,7 @@
       </c>
     </row>
     <row r="302" spans="1:26" ht="12.75">
-      <c r="A302" s="29" t="s">
+      <c r="A302" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B302" s="4" t="s">
@@ -7863,7 +7875,7 @@
       </c>
     </row>
     <row r="303" spans="1:26" ht="12.75">
-      <c r="A303" s="29" t="s">
+      <c r="A303" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B303" s="4" t="s">
@@ -7877,7 +7889,7 @@
       </c>
     </row>
     <row r="304" spans="1:26" ht="12.75">
-      <c r="A304" s="29" t="s">
+      <c r="A304" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B304" s="4" t="s">
@@ -7891,7 +7903,7 @@
       </c>
     </row>
     <row r="305" spans="1:4" ht="12.75">
-      <c r="A305" s="29" t="s">
+      <c r="A305" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B305" s="4" t="s">
@@ -7905,7 +7917,7 @@
       </c>
     </row>
     <row r="306" spans="1:4" ht="12.75">
-      <c r="A306" s="28" t="s">
+      <c r="A306" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B306" s="9" t="s">
@@ -7919,7 +7931,7 @@
       </c>
     </row>
     <row r="307" spans="1:4" ht="12.75">
-      <c r="A307" s="29" t="s">
+      <c r="A307" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B307" s="4" t="s">
@@ -7933,7 +7945,7 @@
       </c>
     </row>
     <row r="308" spans="1:4" ht="12.75">
-      <c r="A308" s="29" t="s">
+      <c r="A308" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B308" s="4" t="s">
@@ -7947,7 +7959,7 @@
       </c>
     </row>
     <row r="309" spans="1:4" ht="12.75">
-      <c r="A309" s="29" t="s">
+      <c r="A309" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B309" s="4" t="s">
@@ -7961,7 +7973,7 @@
       </c>
     </row>
     <row r="310" spans="1:4" ht="12.75">
-      <c r="A310" s="29" t="s">
+      <c r="A310" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B310" s="4" t="s">
@@ -7975,7 +7987,7 @@
       </c>
     </row>
     <row r="311" spans="1:4" ht="12.75">
-      <c r="A311" s="28" t="s">
+      <c r="A311" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B311" s="2" t="s">
@@ -7989,7 +8001,7 @@
       </c>
     </row>
     <row r="312" spans="1:4" ht="12.75">
-      <c r="A312" s="29" t="s">
+      <c r="A312" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B312" s="4" t="s">
@@ -8003,7 +8015,7 @@
       </c>
     </row>
     <row r="313" spans="1:4" ht="12.75">
-      <c r="A313" s="29" t="s">
+      <c r="A313" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B313" s="4" t="s">
@@ -8017,7 +8029,7 @@
       </c>
     </row>
     <row r="314" spans="1:4" ht="12.75">
-      <c r="A314" s="29" t="s">
+      <c r="A314" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B314" s="4" t="s">
@@ -8031,7 +8043,7 @@
       </c>
     </row>
     <row r="315" spans="1:4" ht="12.75">
-      <c r="A315" s="29" t="s">
+      <c r="A315" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B315" s="5" t="s">
@@ -8045,7 +8057,7 @@
       </c>
     </row>
     <row r="316" spans="1:4" ht="12.75">
-      <c r="A316" s="29" t="s">
+      <c r="A316" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B316" s="4" t="s">
@@ -8059,7 +8071,7 @@
       </c>
     </row>
     <row r="317" spans="1:4" ht="12.75">
-      <c r="A317" s="29" t="s">
+      <c r="A317" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B317" s="4" t="s">
@@ -8073,7 +8085,7 @@
       </c>
     </row>
     <row r="318" spans="1:4" ht="12.75">
-      <c r="A318" s="29" t="s">
+      <c r="A318" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B318" s="4" t="s">
@@ -8087,7 +8099,7 @@
       </c>
     </row>
     <row r="319" spans="1:4" ht="12.75">
-      <c r="A319" s="28" t="s">
+      <c r="A319" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B319" s="2" t="s">
@@ -8101,7 +8113,7 @@
       </c>
     </row>
     <row r="320" spans="1:4" ht="12.75">
-      <c r="A320" s="28" t="s">
+      <c r="A320" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B320" s="2" t="s">
@@ -8115,7 +8127,7 @@
       </c>
     </row>
     <row r="321" spans="1:26" ht="12.75">
-      <c r="A321" s="29" t="s">
+      <c r="A321" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B321" s="4" t="s">
@@ -8129,7 +8141,7 @@
       </c>
     </row>
     <row r="322" spans="1:26" ht="12.75">
-      <c r="A322" s="29" t="s">
+      <c r="A322" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B322" s="4" t="s">
@@ -8143,7 +8155,7 @@
       </c>
     </row>
     <row r="323" spans="1:26" ht="12.75">
-      <c r="A323" s="28" t="s">
+      <c r="A323" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B323" s="2" t="s">
@@ -8157,7 +8169,7 @@
       </c>
     </row>
     <row r="324" spans="1:26" ht="12.75">
-      <c r="A324" s="29" t="s">
+      <c r="A324" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B324" s="4" t="s">
@@ -8171,7 +8183,7 @@
       </c>
     </row>
     <row r="325" spans="1:26" ht="12.75">
-      <c r="A325" s="29" t="s">
+      <c r="A325" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B325" s="4" t="s">
@@ -8185,7 +8197,7 @@
       </c>
     </row>
     <row r="326" spans="1:26" ht="12.75">
-      <c r="A326" s="29" t="s">
+      <c r="A326" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B326" s="4" t="s">
@@ -8199,7 +8211,7 @@
       </c>
     </row>
     <row r="327" spans="1:26" ht="12.75">
-      <c r="A327" s="29" t="s">
+      <c r="A327" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B327" s="4" t="s">
@@ -8213,7 +8225,7 @@
       </c>
     </row>
     <row r="328" spans="1:26" ht="12.75">
-      <c r="A328" s="29" t="s">
+      <c r="A328" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B328" s="4" t="s">
@@ -8227,7 +8239,7 @@
       </c>
     </row>
     <row r="329" spans="1:26" ht="12.75">
-      <c r="A329" s="29" t="s">
+      <c r="A329" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B329" s="4" t="s">
@@ -8241,7 +8253,7 @@
       </c>
     </row>
     <row r="330" spans="1:26" ht="12.75">
-      <c r="A330" s="29" t="s">
+      <c r="A330" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B330" s="4" t="s">
@@ -8255,7 +8267,7 @@
       </c>
     </row>
     <row r="331" spans="1:26" ht="12.75">
-      <c r="A331" s="29" t="s">
+      <c r="A331" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B331" s="4" t="s">
@@ -8269,7 +8281,7 @@
       </c>
     </row>
     <row r="332" spans="1:26" ht="12.75">
-      <c r="A332" s="29" t="s">
+      <c r="A332" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B332" s="4" t="s">
@@ -8283,7 +8295,7 @@
       </c>
     </row>
     <row r="333" spans="1:26" ht="12.75">
-      <c r="A333" s="29" t="s">
+      <c r="A333" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B333" s="4" t="s">
@@ -8302,7 +8314,7 @@
       <c r="Z333" s="2"/>
     </row>
     <row r="334" spans="1:26" ht="12.75">
-      <c r="A334" s="29" t="s">
+      <c r="A334" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B334" s="4" t="s">
@@ -8316,7 +8328,7 @@
       </c>
     </row>
     <row r="335" spans="1:26" ht="12.75">
-      <c r="A335" s="28" t="s">
+      <c r="A335" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B335" s="2" t="s">
@@ -8330,7 +8342,7 @@
       </c>
     </row>
     <row r="336" spans="1:26" ht="12.75">
-      <c r="A336" s="29" t="s">
+      <c r="A336" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B336" s="4" t="s">
@@ -8344,7 +8356,7 @@
       </c>
     </row>
     <row r="337" spans="1:4" ht="12.75">
-      <c r="A337" s="29" t="s">
+      <c r="A337" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B337" s="4" t="s">
@@ -8358,7 +8370,7 @@
       </c>
     </row>
     <row r="338" spans="1:4" ht="12.75">
-      <c r="A338" s="29" t="s">
+      <c r="A338" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B338" s="4" t="s">
@@ -8372,7 +8384,7 @@
       </c>
     </row>
     <row r="339" spans="1:4" ht="12.75">
-      <c r="A339" s="29" t="s">
+      <c r="A339" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B339" s="4" t="s">
@@ -8386,7 +8398,7 @@
       </c>
     </row>
     <row r="340" spans="1:4" ht="12.75">
-      <c r="A340" s="29" t="s">
+      <c r="A340" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B340" s="4" t="s">
@@ -8400,7 +8412,7 @@
       </c>
     </row>
     <row r="341" spans="1:4" ht="12.75">
-      <c r="A341" s="29" t="s">
+      <c r="A341" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B341" s="4" t="s">
@@ -8414,7 +8426,7 @@
       </c>
     </row>
     <row r="342" spans="1:4" ht="12.75">
-      <c r="A342" s="29" t="s">
+      <c r="A342" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B342" s="4" t="s">
@@ -8428,7 +8440,7 @@
       </c>
     </row>
     <row r="343" spans="1:4" ht="12.75">
-      <c r="A343" s="29" t="s">
+      <c r="A343" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B343" s="4" t="s">
@@ -8442,7 +8454,7 @@
       </c>
     </row>
     <row r="344" spans="1:4" ht="12.75">
-      <c r="A344" s="28" t="s">
+      <c r="A344" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B344" s="2" t="s">
@@ -8456,7 +8468,7 @@
       </c>
     </row>
     <row r="345" spans="1:4" ht="12.75">
-      <c r="A345" s="28" t="s">
+      <c r="A345" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B345" s="2" t="s">
@@ -8470,7 +8482,7 @@
       </c>
     </row>
     <row r="346" spans="1:4" ht="12.75">
-      <c r="A346" s="29" t="s">
+      <c r="A346" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B346" s="4" t="s">
@@ -8484,7 +8496,7 @@
       </c>
     </row>
     <row r="347" spans="1:4" ht="12.75">
-      <c r="A347" s="29" t="s">
+      <c r="A347" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B347" s="4" t="s">
@@ -8498,7 +8510,7 @@
       </c>
     </row>
     <row r="348" spans="1:4" ht="12.75">
-      <c r="A348" s="29" t="s">
+      <c r="A348" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B348" s="4" t="s">
@@ -8512,7 +8524,7 @@
       </c>
     </row>
     <row r="349" spans="1:4" ht="12.75">
-      <c r="A349" s="29" t="s">
+      <c r="A349" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B349" s="4" t="s">
@@ -8526,7 +8538,7 @@
       </c>
     </row>
     <row r="350" spans="1:4" ht="12.75">
-      <c r="A350" s="29" t="s">
+      <c r="A350" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B350" s="4" t="s">
@@ -8540,7 +8552,7 @@
       </c>
     </row>
     <row r="351" spans="1:4" ht="12.75">
-      <c r="A351" s="29" t="s">
+      <c r="A351" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B351" s="4" t="s">
@@ -8554,7 +8566,7 @@
       </c>
     </row>
     <row r="352" spans="1:4" ht="12.75">
-      <c r="A352" s="28" t="s">
+      <c r="A352" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B352" s="2" t="s">
@@ -8568,7 +8580,7 @@
       </c>
     </row>
     <row r="353" spans="1:4" ht="12.75">
-      <c r="A353" s="28" t="s">
+      <c r="A353" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B353" s="2" t="s">
@@ -8582,7 +8594,7 @@
       </c>
     </row>
     <row r="354" spans="1:4" ht="12.75">
-      <c r="A354" s="28" t="s">
+      <c r="A354" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B354" s="3" t="s">
@@ -8596,7 +8608,7 @@
       </c>
     </row>
     <row r="355" spans="1:4" ht="12.75">
-      <c r="A355" s="29" t="s">
+      <c r="A355" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B355" s="4" t="s">
@@ -8610,7 +8622,7 @@
       </c>
     </row>
     <row r="356" spans="1:4" ht="12.75">
-      <c r="A356" s="28" t="s">
+      <c r="A356" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B356" s="2" t="s">
@@ -8624,7 +8636,7 @@
       </c>
     </row>
     <row r="357" spans="1:4" ht="12.75">
-      <c r="A357" s="28" t="s">
+      <c r="A357" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B357" s="3" t="s">
@@ -8638,7 +8650,7 @@
       </c>
     </row>
     <row r="358" spans="1:4" ht="12.75">
-      <c r="A358" s="29" t="s">
+      <c r="A358" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B358" s="4" t="s">
@@ -8652,7 +8664,7 @@
       </c>
     </row>
     <row r="359" spans="1:4" ht="12.75">
-      <c r="A359" s="29" t="s">
+      <c r="A359" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B359" s="4" t="s">
@@ -8666,7 +8678,7 @@
       </c>
     </row>
     <row r="360" spans="1:4" ht="12.75">
-      <c r="A360" s="29" t="s">
+      <c r="A360" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B360" s="4" t="s">
@@ -8680,7 +8692,7 @@
       </c>
     </row>
     <row r="361" spans="1:4" ht="12.75">
-      <c r="A361" s="29" t="s">
+      <c r="A361" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B361" s="4" t="s">
@@ -8694,7 +8706,7 @@
       </c>
     </row>
     <row r="362" spans="1:4" ht="12.75">
-      <c r="A362" s="29" t="s">
+      <c r="A362" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B362" s="4" t="s">
@@ -8708,7 +8720,7 @@
       </c>
     </row>
     <row r="363" spans="1:4" ht="12.75">
-      <c r="A363" s="29" t="s">
+      <c r="A363" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B363" s="4" t="s">
@@ -8722,7 +8734,7 @@
       </c>
     </row>
     <row r="364" spans="1:4" ht="12.75">
-      <c r="A364" s="28" t="s">
+      <c r="A364" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B364" s="2" t="s">
@@ -8736,7 +8748,7 @@
       </c>
     </row>
     <row r="365" spans="1:4" ht="12.75">
-      <c r="A365" s="28" t="s">
+      <c r="A365" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B365" s="2" t="s">
@@ -8750,7 +8762,7 @@
       </c>
     </row>
     <row r="366" spans="1:4" ht="12.75">
-      <c r="A366" s="29" t="s">
+      <c r="A366" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B366" s="4" t="s">
@@ -8764,7 +8776,7 @@
       </c>
     </row>
     <row r="367" spans="1:4" ht="12.75">
-      <c r="A367" s="29" t="s">
+      <c r="A367" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B367" s="4" t="s">
@@ -8778,7 +8790,7 @@
       </c>
     </row>
     <row r="368" spans="1:4" ht="12.75">
-      <c r="A368" s="29" t="s">
+      <c r="A368" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B368" s="4" t="s">
@@ -8792,7 +8804,7 @@
       </c>
     </row>
     <row r="369" spans="1:4" ht="12.75">
-      <c r="A369" s="28" t="s">
+      <c r="A369" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B369" s="2" t="s">
@@ -8806,7 +8818,7 @@
       </c>
     </row>
     <row r="370" spans="1:4" ht="12.75">
-      <c r="A370" s="29" t="s">
+      <c r="A370" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B370" s="4" t="s">
@@ -8820,7 +8832,7 @@
       </c>
     </row>
     <row r="371" spans="1:4" ht="12.75">
-      <c r="A371" s="29" t="s">
+      <c r="A371" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B371" s="4" t="s">
@@ -8834,7 +8846,7 @@
       </c>
     </row>
     <row r="372" spans="1:4" ht="12.75">
-      <c r="A372" s="29" t="s">
+      <c r="A372" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B372" s="4" t="s">
@@ -8848,7 +8860,7 @@
       </c>
     </row>
     <row r="373" spans="1:4" ht="12.75">
-      <c r="A373" s="29" t="s">
+      <c r="A373" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B373" s="4" t="s">
@@ -8862,7 +8874,7 @@
       </c>
     </row>
     <row r="374" spans="1:4" ht="12.75">
-      <c r="A374" s="29" t="s">
+      <c r="A374" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B374" s="4" t="s">
@@ -8876,7 +8888,7 @@
       </c>
     </row>
     <row r="375" spans="1:4" ht="12.75">
-      <c r="A375" s="28" t="s">
+      <c r="A375" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B375" s="2" t="s">
@@ -8890,7 +8902,7 @@
       </c>
     </row>
     <row r="376" spans="1:4" ht="12.75">
-      <c r="A376" s="28" t="s">
+      <c r="A376" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B376" s="2" t="s">
@@ -8904,7 +8916,7 @@
       </c>
     </row>
     <row r="377" spans="1:4" ht="12.75">
-      <c r="A377" s="28" t="s">
+      <c r="A377" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B377" s="2" t="s">
@@ -8918,7 +8930,7 @@
       </c>
     </row>
     <row r="378" spans="1:4" ht="12.75">
-      <c r="A378" s="29" t="s">
+      <c r="A378" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B378" s="4" t="s">
@@ -8932,7 +8944,7 @@
       </c>
     </row>
     <row r="379" spans="1:4" ht="12.75">
-      <c r="A379" s="29" t="s">
+      <c r="A379" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B379" s="4" t="s">
@@ -8946,7 +8958,7 @@
       </c>
     </row>
     <row r="380" spans="1:4" ht="12.75">
-      <c r="A380" s="28" t="s">
+      <c r="A380" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B380" s="2" t="s">
@@ -8960,7 +8972,7 @@
       </c>
     </row>
     <row r="381" spans="1:4" ht="12.75">
-      <c r="A381" s="28" t="s">
+      <c r="A381" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B381" s="2" t="s">
@@ -8974,7 +8986,7 @@
       </c>
     </row>
     <row r="382" spans="1:4" ht="12.75">
-      <c r="A382" s="28" t="s">
+      <c r="A382" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B382" s="9" t="s">
@@ -8988,7 +9000,7 @@
       </c>
     </row>
     <row r="383" spans="1:4" ht="12.75">
-      <c r="A383" s="29" t="s">
+      <c r="A383" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B383" s="10" t="s">
@@ -9002,7 +9014,7 @@
       </c>
     </row>
     <row r="384" spans="1:4" ht="12.75">
-      <c r="A384" s="29" t="s">
+      <c r="A384" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B384" s="10" t="s">
@@ -9016,7 +9028,7 @@
       </c>
     </row>
     <row r="385" spans="1:4" ht="12.75">
-      <c r="A385" s="29" t="s">
+      <c r="A385" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B385" s="10" t="s">
@@ -9030,7 +9042,7 @@
       </c>
     </row>
     <row r="386" spans="1:4" ht="12.75">
-      <c r="A386" s="29" t="s">
+      <c r="A386" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B386" s="10" t="s">
@@ -9044,7 +9056,7 @@
       </c>
     </row>
     <row r="387" spans="1:4" ht="12.75">
-      <c r="A387" s="29" t="s">
+      <c r="A387" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B387" s="10" t="s">
@@ -9058,7 +9070,7 @@
       </c>
     </row>
     <row r="388" spans="1:4" ht="12.75">
-      <c r="A388" s="29" t="s">
+      <c r="A388" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B388" s="10" t="s">
@@ -9072,7 +9084,7 @@
       </c>
     </row>
     <row r="389" spans="1:4" ht="12.75">
-      <c r="A389" s="29" t="s">
+      <c r="A389" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B389" s="10" t="s">
@@ -9086,7 +9098,7 @@
       </c>
     </row>
     <row r="390" spans="1:4" ht="12.75">
-      <c r="A390" s="28" t="s">
+      <c r="A390" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B390" s="9" t="s">
@@ -9100,7 +9112,7 @@
       </c>
     </row>
     <row r="391" spans="1:4" ht="12.75">
-      <c r="A391" s="29" t="s">
+      <c r="A391" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B391" s="10" t="s">
@@ -9114,7 +9126,7 @@
       </c>
     </row>
     <row r="392" spans="1:4" ht="12.75">
-      <c r="A392" s="29" t="s">
+      <c r="A392" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B392" s="10" t="s">
@@ -9128,7 +9140,7 @@
       </c>
     </row>
     <row r="393" spans="1:4" ht="12.75">
-      <c r="A393" s="29" t="s">
+      <c r="A393" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B393" s="10" t="s">
@@ -9142,7 +9154,7 @@
       </c>
     </row>
     <row r="394" spans="1:4" ht="12.75">
-      <c r="A394" s="29" t="s">
+      <c r="A394" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B394" s="10" t="s">
@@ -9156,7 +9168,7 @@
       </c>
     </row>
     <row r="395" spans="1:4" ht="12.75">
-      <c r="A395" s="29" t="s">
+      <c r="A395" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B395" s="10" t="s">
@@ -9170,7 +9182,7 @@
       </c>
     </row>
     <row r="396" spans="1:4" ht="12.75">
-      <c r="A396" s="29" t="s">
+      <c r="A396" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B396" s="10" t="s">
@@ -9184,7 +9196,7 @@
       </c>
     </row>
     <row r="397" spans="1:4" ht="12.75">
-      <c r="A397" s="29" t="s">
+      <c r="A397" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B397" s="10" t="s">
@@ -9198,7 +9210,7 @@
       </c>
     </row>
     <row r="398" spans="1:4" ht="12.75">
-      <c r="A398" s="29" t="s">
+      <c r="A398" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B398" s="10" t="s">
@@ -9212,7 +9224,7 @@
       </c>
     </row>
     <row r="399" spans="1:4" ht="12.75">
-      <c r="A399" s="28" t="s">
+      <c r="A399" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B399" s="9" t="s">
@@ -9226,7 +9238,7 @@
       </c>
     </row>
     <row r="400" spans="1:4" ht="12.75">
-      <c r="A400" s="29" t="s">
+      <c r="A400" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B400" s="10" t="s">
@@ -9240,7 +9252,7 @@
       </c>
     </row>
     <row r="401" spans="1:26" ht="12.75">
-      <c r="A401" s="29" t="s">
+      <c r="A401" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B401" s="10" t="s">
@@ -9254,7 +9266,7 @@
       </c>
     </row>
     <row r="402" spans="1:26" ht="12.75">
-      <c r="A402" s="28" t="s">
+      <c r="A402" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B402" s="9" t="s">
@@ -9268,7 +9280,7 @@
       </c>
     </row>
     <row r="403" spans="1:26" ht="12.75">
-      <c r="A403" s="29" t="s">
+      <c r="A403" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B403" s="24" t="s">
@@ -9304,7 +9316,7 @@
       <c r="Z403" s="6"/>
     </row>
     <row r="404" spans="1:26" ht="12.75">
-      <c r="A404" s="29" t="s">
+      <c r="A404" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B404" s="4" t="s">
@@ -9318,7 +9330,7 @@
       </c>
     </row>
     <row r="405" spans="1:26" ht="12.75">
-      <c r="A405" s="28" t="s">
+      <c r="A405" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B405" s="2" t="s">
@@ -9332,7 +9344,7 @@
       </c>
     </row>
     <row r="406" spans="1:26" ht="12.75">
-      <c r="A406" s="28" t="s">
+      <c r="A406" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B406" s="2" t="s">
@@ -9346,7 +9358,7 @@
       </c>
     </row>
     <row r="407" spans="1:26" ht="12.75">
-      <c r="A407" s="29" t="s">
+      <c r="A407" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B407" s="4" t="s">
@@ -9360,7 +9372,7 @@
       </c>
     </row>
     <row r="408" spans="1:26" ht="12.75">
-      <c r="A408" s="29" t="s">
+      <c r="A408" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B408" s="4" t="s">
@@ -9374,7 +9386,7 @@
       </c>
     </row>
     <row r="409" spans="1:26" ht="12.75">
-      <c r="A409" s="28" t="s">
+      <c r="A409" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B409" s="2" t="s">
@@ -9388,7 +9400,7 @@
       </c>
     </row>
     <row r="410" spans="1:26" ht="12.75">
-      <c r="A410" s="29" t="s">
+      <c r="A410" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B410" s="4" t="s">
@@ -9402,7 +9414,7 @@
       </c>
     </row>
     <row r="411" spans="1:26" ht="12.75">
-      <c r="A411" s="29" t="s">
+      <c r="A411" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B411" s="4" t="s">
@@ -9416,7 +9428,7 @@
       </c>
     </row>
     <row r="412" spans="1:26" ht="12.75">
-      <c r="A412" s="28" t="s">
+      <c r="A412" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B412" s="2" t="s">
@@ -9430,7 +9442,7 @@
       </c>
     </row>
     <row r="413" spans="1:26" ht="12.75">
-      <c r="A413" s="28" t="s">
+      <c r="A413" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B413" s="2" t="s">
@@ -9444,7 +9456,7 @@
       </c>
     </row>
     <row r="414" spans="1:26" ht="12.75">
-      <c r="A414" s="29" t="s">
+      <c r="A414" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B414" s="4" t="s">
@@ -9458,7 +9470,7 @@
       </c>
     </row>
     <row r="415" spans="1:26" ht="12.75">
-      <c r="A415" s="28" t="s">
+      <c r="A415" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B415" s="2" t="s">
@@ -9472,7 +9484,7 @@
       </c>
     </row>
     <row r="416" spans="1:26" ht="12.75">
-      <c r="A416" s="29" t="s">
+      <c r="A416" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B416" s="4" t="s">
@@ -9486,7 +9498,7 @@
       </c>
     </row>
     <row r="417" spans="1:4" ht="12.75">
-      <c r="A417" s="28" t="s">
+      <c r="A417" s="27" t="s">
         <v>533</v>
       </c>
       <c r="B417" s="2" t="s">
@@ -9500,7 +9512,7 @@
       </c>
     </row>
     <row r="418" spans="1:4" ht="12.75">
-      <c r="A418" s="28" t="s">
+      <c r="A418" s="27" t="s">
         <v>530</v>
       </c>
       <c r="B418" s="2" t="s">
@@ -9514,7 +9526,7 @@
       </c>
     </row>
     <row r="419" spans="1:4" ht="12.75">
-      <c r="A419" s="28" t="s">
+      <c r="A419" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B419" s="2" t="s">
@@ -9528,7 +9540,7 @@
       </c>
     </row>
     <row r="420" spans="1:4" ht="12.75">
-      <c r="A420" s="28" t="s">
+      <c r="A420" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B420" s="2" t="s">
@@ -9542,7 +9554,7 @@
       </c>
     </row>
     <row r="421" spans="1:4" ht="12.75">
-      <c r="A421" s="29" t="s">
+      <c r="A421" s="28" t="s">
         <v>748</v>
       </c>
       <c r="B421" s="4" t="s">
@@ -9556,7 +9568,7 @@
       </c>
     </row>
     <row r="422" spans="1:4" ht="12.75">
-      <c r="A422" s="28" t="s">
+      <c r="A422" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B422" s="2" t="s">
@@ -9570,7 +9582,7 @@
       </c>
     </row>
     <row r="423" spans="1:4" ht="12.75">
-      <c r="A423" s="28" t="s">
+      <c r="A423" s="27" t="s">
         <v>748</v>
       </c>
       <c r="B423" s="2" t="s">

</xml_diff>